<commit_message>
Added more emoji to data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fodmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEFC03B-8729-4ED0-9562-9FCA4E3F59B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB315E-FD67-4DA2-8D1F-ED5F082B2FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="285" xr2:uid="{5144C98B-C405-4E2F-B3EA-D69079E9313A}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="473">
   <si>
     <t>Name</t>
   </si>
@@ -568,9 +568,6 @@
     <t>Pasta</t>
   </si>
   <si>
-    <t>No soy or legume flours</t>
-  </si>
-  <si>
     <t>Polenta</t>
   </si>
   <si>
@@ -1087,9 +1084,6 @@
     <t>Herbs &amp; Spices</t>
   </si>
   <si>
-    <t>Check for no onion or garlic in ingredients.</t>
-  </si>
-  <si>
     <t>Strawberry Jam</t>
   </si>
   <si>
@@ -1442,6 +1436,48 @@
   </si>
   <si>
     <t>🍇</t>
+  </si>
+  <si>
+    <t>No soy/legume flours.</t>
+  </si>
+  <si>
+    <t>🥝</t>
+  </si>
+  <si>
+    <t>🍋</t>
+  </si>
+  <si>
+    <t>🍑</t>
+  </si>
+  <si>
+    <t>🍍</t>
+  </si>
+  <si>
+    <t>🍐</t>
+  </si>
+  <si>
+    <t>🍒</t>
+  </si>
+  <si>
+    <t>🫐</t>
+  </si>
+  <si>
+    <t>🍓</t>
+  </si>
+  <si>
+    <t>🍎</t>
+  </si>
+  <si>
+    <t>🍏</t>
+  </si>
+  <si>
+    <t>🥭</t>
+  </si>
+  <si>
+    <t>🍉</t>
+  </si>
+  <si>
+    <t>🌷</t>
   </si>
 </sst>
 </file>
@@ -1852,8 +1888,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D982221-C92D-46DA-BAB2-38212BF311A8}">
   <dimension ref="A1:G377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B351" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G377"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1899,7 @@
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="138.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1881,10 +1918,10 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
@@ -1903,7 +1940,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G2" s="2" t="str">
         <f>CONCATENATE("{ name: "&amp;CHAR(34),A2 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B2&amp;CHAR(34), ", ", "avoid: ", LOWER(C2), ", measurement: "&amp;CHAR(34), D2, CHAR(34), ", notes: ", CHAR(34), E2, CHAR(34), ", emoji: '", F2, "'", " },")</f>
@@ -1923,7 +1960,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G66" si="0">CONCATENATE("{ name: "&amp;CHAR(34),A3 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B3&amp;CHAR(34), ", ", "avoid: ", LOWER(C3), ", measurement: "&amp;CHAR(34), D3, CHAR(34), ", notes: ", CHAR(34), E3, CHAR(34), ", emoji: '", F3, "'", " },")</f>
@@ -1966,7 +2003,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1986,7 +2023,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2029,7 +2066,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2049,7 +2086,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2069,7 +2106,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2091,7 +2128,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2111,7 +2148,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2131,7 +2168,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2151,7 +2188,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2173,7 +2210,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2193,7 +2230,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2213,7 +2250,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2235,7 +2272,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2255,7 +2292,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2273,11 +2310,11 @@
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2299,7 +2336,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2319,7 +2356,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2339,7 +2376,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2359,7 +2396,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2381,7 +2418,7 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2401,7 +2438,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2421,7 +2458,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2441,7 +2478,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2461,7 +2498,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2481,7 +2518,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2503,7 +2540,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2523,7 +2560,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2543,7 +2580,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2563,7 +2600,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2583,7 +2620,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2603,7 +2640,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G36" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2625,7 +2662,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G37" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2645,7 +2682,7 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G38" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2665,7 +2702,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G39" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2685,7 +2722,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G40" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2705,7 +2742,7 @@
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G41" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2725,7 +2762,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G42" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2745,7 +2782,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="G43" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2765,7 +2802,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G44" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2785,7 +2822,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G45" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2805,7 +2842,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2825,7 +2862,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2843,11 +2880,11 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2867,7 +2904,7 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G49" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2887,7 +2924,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G50" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2909,7 +2946,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G51" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2929,7 +2966,7 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G52" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2951,7 +2988,7 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G53" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2971,7 +3008,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G54" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2993,7 +3030,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G55" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3015,7 +3052,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G56" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3035,7 +3072,7 @@
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G57" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3055,7 +3092,7 @@
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G58" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3075,7 +3112,7 @@
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G59" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3093,11 +3130,11 @@
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G60" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3117,7 +3154,7 @@
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G61" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3137,7 +3174,7 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G62" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3157,7 +3194,7 @@
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G63" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3179,7 +3216,7 @@
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G64" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3199,7 +3236,7 @@
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G65" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3219,7 +3256,7 @@
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G66" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3239,7 +3276,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G67" s="2" t="str">
         <f t="shared" ref="G67:G130" si="1">CONCATENATE("{ name: "&amp;CHAR(34),A67 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B67&amp;CHAR(34), ", ", "avoid: ", LOWER(C67), ", measurement: "&amp;CHAR(34), D67, CHAR(34), ", notes: ", CHAR(34), E67, CHAR(34), ", emoji: '", F67, "'", " },")</f>
@@ -3259,7 +3296,7 @@
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G68" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3279,7 +3316,7 @@
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G69" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3299,7 +3336,7 @@
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G70" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3319,7 +3356,7 @@
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G71" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3339,7 +3376,7 @@
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G72" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3359,7 +3396,7 @@
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G73" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3379,7 +3416,7 @@
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G74" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3399,7 +3436,7 @@
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G75" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3419,7 +3456,7 @@
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G76" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3439,7 +3476,7 @@
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G77" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3461,7 +3498,7 @@
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G78" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3483,7 +3520,7 @@
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G79" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3503,7 +3540,7 @@
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G80" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3521,11 +3558,11 @@
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G81" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3547,7 +3584,7 @@
       </c>
       <c r="E82" s="2"/>
       <c r="F82" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G82" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3569,7 +3606,7 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="G83" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3589,7 +3626,7 @@
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G84" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3609,7 +3646,7 @@
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G85" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3629,7 +3666,7 @@
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G86" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3649,7 +3686,7 @@
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G87" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3690,7 +3727,7 @@
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G89" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3712,7 +3749,7 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G90" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3734,7 +3771,7 @@
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G91" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3754,7 +3791,7 @@
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G92" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3776,7 +3813,7 @@
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G93" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3798,7 +3835,7 @@
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G94" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3820,7 +3857,7 @@
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G95" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3840,7 +3877,7 @@
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G96" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3860,7 +3897,7 @@
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G97" s="2" t="str">
         <f t="shared" si="1"/>
@@ -3879,10 +3916,12 @@
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
+      <c r="F98" s="2" t="s">
+        <v>458</v>
+      </c>
       <c r="G98" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Guava", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Guava", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍇' },</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3897,10 +3936,12 @@
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
+      <c r="F99" s="2" t="s">
+        <v>440</v>
+      </c>
       <c r="G99" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Jackfruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Jackfruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍈' },</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3915,10 +3956,12 @@
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
+      <c r="F100" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="G100" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Kiwifruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Kiwifruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🥝' },</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3933,10 +3976,12 @@
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
+      <c r="F101" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="G101" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Lemon", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lemon", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍋' },</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3951,10 +3996,12 @@
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
+      <c r="F102" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="G102" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Lime", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lime", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍋' },</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3969,10 +4016,12 @@
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
+      <c r="F103" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="G103" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Mandarin", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mandarin", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3987,10 +4036,12 @@
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
+      <c r="F104" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="G104" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "White Nectarine", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "White Nectarine", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍑' },</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4005,10 +4056,12 @@
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
+      <c r="F105" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="G105" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Orange", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Orange", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4023,10 +4076,12 @@
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
+      <c r="F106" s="2" t="s">
+        <v>440</v>
+      </c>
       <c r="G106" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Passionfruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Passionfruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍈' },</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4041,10 +4096,12 @@
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
+      <c r="F107" s="2" t="s">
+        <v>463</v>
+      </c>
       <c r="G107" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Pineapple", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pineapple", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍍' },</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4061,10 +4118,12 @@
         <v>29</v>
       </c>
       <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>440</v>
+      </c>
       <c r="G108" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Pomegranate", category: "Fruit", avoid: false, measurement: "¼ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Pomegranate", category: "Fruit", avoid: false, measurement: "¼ cup", notes: "", emoji: '🍈' },</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4079,10 +4138,12 @@
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="G109" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Prickly Pear", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Prickly Pear", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍐' },</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4099,10 +4160,12 @@
         <v>129</v>
       </c>
       <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
+      <c r="F110" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="G110" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Rambutan", category: "Fruit", avoid: false, measurement: "Up to 3", notes: "", emoji: '' },</v>
+        <v>{ name: "Rambutan", category: "Fruit", avoid: false, measurement: "Up to 3", notes: "", emoji: '🍒' },</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4117,10 +4180,12 @@
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
+      <c r="F111" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="G111" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Raspberries", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Raspberries", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🫐' },</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4135,10 +4200,12 @@
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
+      <c r="F112" s="2" t="s">
+        <v>440</v>
+      </c>
       <c r="G112" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Rhubarb", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rhubarb", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍈' },</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4153,10 +4220,12 @@
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
+      <c r="F113" s="2" t="s">
+        <v>455</v>
+      </c>
       <c r="G113" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Star Fruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Star Fruit", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '⭐' },</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4171,10 +4240,12 @@
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
+      <c r="F114" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="G114" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Strawberries", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Strawberries", category: "Fruit", avoid: false, measurement: "", notes: "", emoji: '🍓' },</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4189,10 +4260,12 @@
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>468</v>
+      </c>
       <c r="G115" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Apple", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Apple", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍎' },</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4207,10 +4280,12 @@
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="G116" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Fresh Apricot", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fresh Apricot", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4225,10 +4300,12 @@
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
+      <c r="F117" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="G117" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Dried Apricot", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Dried Apricot", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4245,10 +4322,12 @@
         <v>137</v>
       </c>
       <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
+      <c r="F118" s="2" t="s">
+        <v>453</v>
+      </c>
       <c r="G118" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Banana", category: "Fruit", avoid: true, measurement: "Ripe", notes: "", emoji: '' },</v>
+        <v>{ name: "Banana", category: "Fruit", avoid: true, measurement: "Ripe", notes: "", emoji: '🍌' },</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4262,10 +4341,12 @@
         <v>1</v>
       </c>
       <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
+      <c r="F119" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="G119" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Blackberries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Blackberries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🫐' },</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4280,10 +4361,12 @@
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
+      <c r="F120" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="G120" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Boysenberries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Boysenberries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🫐' },</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4298,10 +4381,12 @@
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
+      <c r="F121" s="2" t="s">
+        <v>465</v>
+      </c>
       <c r="G121" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Cherries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cherries", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍒' },</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4316,10 +4401,12 @@
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
+      <c r="F122" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="G122" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Custard Apple", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Custard Apple", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍏' },</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4334,10 +4421,12 @@
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
+      <c r="F123" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="G123" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Feijoa", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Feijoa", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍏' },</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4352,10 +4441,12 @@
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
+      <c r="F124" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="G124" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Mango", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mango", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🥭' },</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4370,10 +4461,12 @@
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
+      <c r="F125" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="G125" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Nectarine", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Nectarine", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍑' },</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4388,10 +4481,12 @@
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
+      <c r="F126" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="G126" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Peach", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Peach", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍑' },</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4406,10 +4501,12 @@
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
+      <c r="F127" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="G127" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Pear", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pear", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍐' },</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4424,10 +4521,12 @@
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
+      <c r="F128" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="G128" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Persimmon", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Persimmon", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍅' },</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4442,10 +4541,12 @@
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
+      <c r="F129" s="2" t="s">
+        <v>453</v>
+      </c>
       <c r="G129" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Sugar Banana", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Sugar Banana", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍌' },</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4460,10 +4561,12 @@
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
+      <c r="F130" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="G130" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>{ name: "Tamarillo", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Tamarillo", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍅' },</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4478,10 +4581,12 @@
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
+      <c r="F131" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="G131" s="2" t="str">
         <f t="shared" ref="G131:G194" si="2">CONCATENATE("{ name: "&amp;CHAR(34),A131 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B131&amp;CHAR(34), ", ", "avoid: ", LOWER(C131), ", measurement: "&amp;CHAR(34), D131, CHAR(34), ", notes: ", CHAR(34), E131, CHAR(34), ", emoji: '", F131, "'", " },")</f>
-        <v>{ name: "Watermelon", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Watermelon", category: "Fruit", avoid: true, measurement: "", notes: "", emoji: '🍉' },</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4498,10 +4603,12 @@
         <v>153</v>
       </c>
       <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
+      <c r="F132" s="5" t="s">
+        <v>472</v>
+      </c>
       <c r="G132" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Amaranth", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "¼ cup puffed, not flour", notes: "", emoji: '' },</v>
+        <v>{ name: "Amaranth", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "¼ cup puffed, not flour", notes: "", emoji: '🌷' },</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4516,10 +4623,12 @@
       </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
+      <c r="F133" s="2" t="s">
+        <v>438</v>
+      </c>
       <c r="G133" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Arrowroot", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Arrowroot", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🍠' },</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4589,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
@@ -4772,17 +4881,17 @@
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2" t="s">
-        <v>169</v>
+        <v>459</v>
       </c>
       <c r="F147" s="2"/>
       <c r="G147" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "No soy or legume flours", emoji: '' },</v>
+        <v>{ name: "Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "No soy/legume flours.", emoji: '' },</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>151</v>
@@ -4800,7 +4909,7 @@
     </row>
     <row r="149" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>151</v>
@@ -4818,7 +4927,7 @@
     </row>
     <row r="150" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>151</v>
@@ -4836,7 +4945,7 @@
     </row>
     <row r="151" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>151</v>
@@ -4854,7 +4963,7 @@
     </row>
     <row r="152" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>151</v>
@@ -4872,7 +4981,7 @@
     </row>
     <row r="153" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>151</v>
@@ -4890,7 +4999,7 @@
     </row>
     <row r="154" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>151</v>
@@ -4908,7 +5017,7 @@
     </row>
     <row r="155" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>151</v>
@@ -4928,7 +5037,7 @@
     </row>
     <row r="156" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>151</v>
@@ -4937,7 +5046,7 @@
         <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E156" s="2"/>
       <c r="F156" s="2"/>
@@ -4948,7 +5057,7 @@
     </row>
     <row r="157" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>151</v>
@@ -4968,7 +5077,7 @@
     </row>
     <row r="158" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>151</v>
@@ -4977,7 +5086,7 @@
         <v>0</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E158" s="2"/>
       <c r="F158" s="2"/>
@@ -4988,7 +5097,7 @@
     </row>
     <row r="159" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B159" s="2" t="s">
         <v>151</v>
@@ -5008,7 +5117,7 @@
     </row>
     <row r="160" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>151</v>
@@ -5026,7 +5135,7 @@
     </row>
     <row r="161" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>151</v>
@@ -5044,7 +5153,7 @@
     </row>
     <row r="162" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>151</v>
@@ -5062,7 +5171,7 @@
     </row>
     <row r="163" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>151</v>
@@ -5080,7 +5189,7 @@
     </row>
     <row r="164" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B164" s="2" t="s">
         <v>151</v>
@@ -5098,7 +5207,7 @@
     </row>
     <row r="165" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>151</v>
@@ -5116,7 +5225,7 @@
     </row>
     <row r="166" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B166" s="2" t="s">
         <v>151</v>
@@ -5134,7 +5243,7 @@
     </row>
     <row r="167" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>151</v>
@@ -5152,7 +5261,7 @@
     </row>
     <row r="168" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>151</v>
@@ -5170,7 +5279,7 @@
     </row>
     <row r="169" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B169" s="2" t="s">
         <v>151</v>
@@ -5188,7 +5297,7 @@
     </row>
     <row r="170" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>151</v>
@@ -5206,7 +5315,7 @@
     </row>
     <row r="171" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B171" s="2" t="s">
         <v>151</v>
@@ -5224,7 +5333,7 @@
     </row>
     <row r="172" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B172" s="2" t="s">
         <v>151</v>
@@ -5242,7 +5351,7 @@
     </row>
     <row r="173" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>151</v>
@@ -5260,7 +5369,7 @@
     </row>
     <row r="174" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B174" s="2" t="s">
         <v>151</v>
@@ -5278,7 +5387,7 @@
     </row>
     <row r="175" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B175" s="2" t="s">
         <v>151</v>
@@ -5296,7 +5405,7 @@
     </row>
     <row r="176" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B176" s="2" t="s">
         <v>151</v>
@@ -5314,7 +5423,7 @@
     </row>
     <row r="177" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B177" s="2" t="s">
         <v>151</v>
@@ -5332,7 +5441,7 @@
     </row>
     <row r="178" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B178" s="2" t="s">
         <v>151</v>
@@ -5350,7 +5459,7 @@
     </row>
     <row r="179" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B179" s="2" t="s">
         <v>151</v>
@@ -5368,7 +5477,7 @@
     </row>
     <row r="180" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B180" s="2" t="s">
         <v>151</v>
@@ -5386,7 +5495,7 @@
     </row>
     <row r="181" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B181" s="2" t="s">
         <v>151</v>
@@ -5404,7 +5513,7 @@
     </row>
     <row r="182" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>151</v>
@@ -5422,7 +5531,7 @@
     </row>
     <row r="183" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>151</v>
@@ -5440,7 +5549,7 @@
     </row>
     <row r="184" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>151</v>
@@ -5458,7 +5567,7 @@
     </row>
     <row r="185" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>151</v>
@@ -5476,7 +5585,7 @@
     </row>
     <row r="186" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B186" s="2" t="s">
         <v>151</v>
@@ -5494,7 +5603,7 @@
     </row>
     <row r="187" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B187" s="2" t="s">
         <v>151</v>
@@ -5512,7 +5621,7 @@
     </row>
     <row r="188" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B188" s="2" t="s">
         <v>151</v>
@@ -5530,7 +5639,7 @@
     </row>
     <row r="189" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B189" s="2" t="s">
         <v>151</v>
@@ -5548,7 +5657,7 @@
     </row>
     <row r="190" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>151</v>
@@ -5566,7 +5675,7 @@
     </row>
     <row r="191" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>151</v>
@@ -5584,10 +5693,10 @@
     </row>
     <row r="192" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C192" s="2" t="b">
         <v>0</v>
@@ -5602,16 +5711,16 @@
     </row>
     <row r="193" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C193" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
@@ -5622,10 +5731,10 @@
     </row>
     <row r="194" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C194" s="2" t="b">
         <v>0</v>
@@ -5640,10 +5749,10 @@
     </row>
     <row r="195" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C195" s="2" t="b">
         <v>0</v>
@@ -5658,10 +5767,10 @@
     </row>
     <row r="196" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C196" s="2" t="b">
         <v>0</v>
@@ -5676,10 +5785,10 @@
     </row>
     <row r="197" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C197" s="2" t="b">
         <v>0</v>
@@ -5694,16 +5803,16 @@
     </row>
     <row r="198" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C198" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
@@ -5714,16 +5823,16 @@
     </row>
     <row r="199" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C199" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
@@ -5734,16 +5843,16 @@
     </row>
     <row r="200" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C200" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
@@ -5754,10 +5863,10 @@
     </row>
     <row r="201" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C201" s="2" t="b">
         <v>1</v>
@@ -5772,10 +5881,10 @@
     </row>
     <row r="202" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C202" s="2" t="b">
         <v>1</v>
@@ -5790,10 +5899,10 @@
     </row>
     <row r="203" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C203" s="2" t="b">
         <v>1</v>
@@ -5808,10 +5917,10 @@
     </row>
     <row r="204" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C204" s="2" t="b">
         <v>1</v>
@@ -5826,10 +5935,10 @@
     </row>
     <row r="205" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C205" s="2" t="b">
         <v>1</v>
@@ -5844,10 +5953,10 @@
     </row>
     <row r="206" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C206" s="2" t="b">
         <v>0</v>
@@ -5862,10 +5971,10 @@
     </row>
     <row r="207" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C207" s="2" t="b">
         <v>0</v>
@@ -5880,10 +5989,10 @@
     </row>
     <row r="208" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C208" s="2" t="b">
         <v>0</v>
@@ -5898,10 +6007,10 @@
     </row>
     <row r="209" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C209" s="2" t="b">
         <v>0</v>
@@ -5916,10 +6025,10 @@
     </row>
     <row r="210" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C210" s="2" t="b">
         <v>0</v>
@@ -5936,10 +6045,10 @@
     </row>
     <row r="211" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C211" s="2" t="b">
         <v>0</v>
@@ -5956,10 +6065,10 @@
     </row>
     <row r="212" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C212" s="2" t="b">
         <v>0</v>
@@ -5974,17 +6083,17 @@
     </row>
     <row r="213" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C213" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D213" s="2"/>
       <c r="E213" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F213" s="2"/>
       <c r="G213" s="2" t="str">
@@ -5994,17 +6103,17 @@
     </row>
     <row r="214" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C214" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D214" s="2"/>
       <c r="E214" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F214" s="2"/>
       <c r="G214" s="2" t="str">
@@ -6014,16 +6123,16 @@
     </row>
     <row r="215" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C215" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D215" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C215" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D215" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="E215" s="5"/>
       <c r="F215" s="5"/>
@@ -6034,17 +6143,17 @@
     </row>
     <row r="216" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C216" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D216" s="2"/>
       <c r="E216" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2" t="str">
@@ -6054,16 +6163,16 @@
     </row>
     <row r="217" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C217" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E217" s="2"/>
       <c r="F217" s="2"/>
@@ -6074,16 +6183,16 @@
     </row>
     <row r="218" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C218" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E218" s="2"/>
       <c r="F218" s="2"/>
@@ -6094,16 +6203,16 @@
     </row>
     <row r="219" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C219" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E219" s="2"/>
       <c r="F219" s="2"/>
@@ -6114,16 +6223,16 @@
     </row>
     <row r="220" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C220" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E220" s="2"/>
       <c r="F220" s="2"/>
@@ -6134,16 +6243,16 @@
     </row>
     <row r="221" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C221" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E221" s="2"/>
       <c r="F221" s="2"/>
@@ -6154,16 +6263,16 @@
     </row>
     <row r="222" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C222" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E222" s="2"/>
       <c r="F222" s="2"/>
@@ -6174,16 +6283,16 @@
     </row>
     <row r="223" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C223" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E223" s="2"/>
       <c r="F223" s="2"/>
@@ -6194,16 +6303,16 @@
     </row>
     <row r="224" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C224" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E224" s="2"/>
       <c r="F224" s="2"/>
@@ -6214,16 +6323,16 @@
     </row>
     <row r="225" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C225" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E225" s="2"/>
       <c r="F225" s="2"/>
@@ -6234,16 +6343,16 @@
     </row>
     <row r="226" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C226" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D226" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E226" s="5"/>
       <c r="F226" s="5"/>
@@ -6254,16 +6363,16 @@
     </row>
     <row r="227" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C227" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
@@ -6274,16 +6383,16 @@
     </row>
     <row r="228" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C228" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
@@ -6294,16 +6403,16 @@
     </row>
     <row r="229" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C229" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D229" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E229" s="5"/>
       <c r="F229" s="5"/>
@@ -6314,16 +6423,16 @@
     </row>
     <row r="230" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C230" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
@@ -6334,16 +6443,16 @@
     </row>
     <row r="231" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C231" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
@@ -6354,10 +6463,10 @@
     </row>
     <row r="232" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C232" s="2" t="b">
         <v>1</v>
@@ -6375,7 +6484,7 @@
         <v>101</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C233" s="2" t="b">
         <v>1</v>
@@ -6390,10 +6499,10 @@
     </row>
     <row r="234" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C234" s="2" t="b">
         <v>1</v>
@@ -6408,10 +6517,10 @@
     </row>
     <row r="235" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C235" s="2" t="b">
         <v>1</v>
@@ -6426,10 +6535,10 @@
     </row>
     <row r="236" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C236" s="2" t="b">
         <v>1</v>
@@ -6444,10 +6553,10 @@
     </row>
     <row r="237" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C237" s="2" t="b">
         <v>1</v>
@@ -6462,10 +6571,10 @@
     </row>
     <row r="238" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C238" s="2" t="b">
         <v>1</v>
@@ -6480,10 +6589,10 @@
     </row>
     <row r="239" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C239" s="2" t="b">
         <v>1</v>
@@ -6498,16 +6607,16 @@
     </row>
     <row r="240" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B240" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C240" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D240" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C240" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E240" s="2"/>
       <c r="F240" s="2"/>
@@ -6518,16 +6627,16 @@
     </row>
     <row r="241" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B241" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C241" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D241" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C241" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E241" s="2"/>
       <c r="F241" s="2"/>
@@ -6538,16 +6647,16 @@
     </row>
     <row r="242" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B242" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C242" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D242" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C242" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E242" s="2"/>
       <c r="F242" s="2"/>
@@ -6558,16 +6667,16 @@
     </row>
     <row r="243" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B243" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C243" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D243" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C243" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E243" s="2"/>
       <c r="F243" s="2"/>
@@ -6578,16 +6687,16 @@
     </row>
     <row r="244" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B244" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C244" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D244" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C244" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E244" s="2"/>
       <c r="F244" s="2"/>
@@ -6598,16 +6707,16 @@
     </row>
     <row r="245" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B245" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C245" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D245" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C245" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D245" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E245" s="2"/>
       <c r="F245" s="2"/>
@@ -6618,16 +6727,16 @@
     </row>
     <row r="246" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B246" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C246" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D246" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C246" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
@@ -6638,16 +6747,16 @@
     </row>
     <row r="247" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B247" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C247" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D247" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C247" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
@@ -6658,16 +6767,16 @@
     </row>
     <row r="248" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B248" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C248" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D248" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C248" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D248" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
@@ -6678,16 +6787,16 @@
     </row>
     <row r="249" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B249" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C249" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D249" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C249" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E249" s="2"/>
       <c r="F249" s="2"/>
@@ -6698,16 +6807,16 @@
     </row>
     <row r="250" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B250" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C250" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D250" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C250" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
@@ -6718,16 +6827,16 @@
     </row>
     <row r="251" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B251" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C251" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D251" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C251" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
@@ -6738,16 +6847,16 @@
     </row>
     <row r="252" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B252" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C252" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D252" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C252" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D252" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E252" s="2"/>
       <c r="F252" s="2"/>
@@ -6758,10 +6867,10 @@
     </row>
     <row r="253" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C253" s="2" t="b">
         <v>0</v>
@@ -6778,10 +6887,10 @@
     </row>
     <row r="254" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C254" s="2" t="b">
         <v>0</v>
@@ -6798,10 +6907,10 @@
     </row>
     <row r="255" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C255" s="2" t="b">
         <v>0</v>
@@ -6818,10 +6927,10 @@
     </row>
     <row r="256" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C256" s="2" t="b">
         <v>0</v>
@@ -6838,16 +6947,16 @@
     </row>
     <row r="257" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C257" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E257" s="5"/>
       <c r="F257" s="5"/>
@@ -6858,10 +6967,10 @@
     </row>
     <row r="258" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C258" s="2" t="b">
         <v>0</v>
@@ -6870,7 +6979,7 @@
         <v>29</v>
       </c>
       <c r="E258" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F258" s="2"/>
       <c r="G258" s="2" t="str">
@@ -6880,10 +6989,10 @@
     </row>
     <row r="259" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C259" s="2" t="b">
         <v>0</v>
@@ -6892,7 +7001,7 @@
         <v>29</v>
       </c>
       <c r="E259" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F259" s="2"/>
       <c r="G259" s="2" t="str">
@@ -6902,10 +7011,10 @@
     </row>
     <row r="260" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C260" s="2" t="b">
         <v>0</v>
@@ -6920,10 +7029,10 @@
     </row>
     <row r="261" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C261" s="2" t="b">
         <v>1</v>
@@ -6938,10 +7047,10 @@
     </row>
     <row r="262" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C262" s="2" t="b">
         <v>1</v>
@@ -6956,10 +7065,10 @@
     </row>
     <row r="263" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C263" s="2" t="b">
         <v>1</v>
@@ -6974,10 +7083,10 @@
     </row>
     <row r="264" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C264" s="2" t="b">
         <v>1</v>
@@ -6992,10 +7101,10 @@
     </row>
     <row r="265" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C265" s="2" t="b">
         <v>1</v>
@@ -7010,10 +7119,10 @@
     </row>
     <row r="266" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C266" s="2" t="b">
         <v>1</v>
@@ -7028,10 +7137,10 @@
     </row>
     <row r="267" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C267" s="2" t="b">
         <v>1</v>
@@ -7046,10 +7155,10 @@
     </row>
     <row r="268" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C268" s="2" t="b">
         <v>1</v>
@@ -7064,10 +7173,10 @@
     </row>
     <row r="269" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C269" s="2" t="b">
         <v>1</v>
@@ -7082,10 +7191,10 @@
     </row>
     <row r="270" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C270" s="2" t="b">
         <v>1</v>
@@ -7100,10 +7209,10 @@
     </row>
     <row r="271" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C271" s="2" t="b">
         <v>1</v>
@@ -7118,10 +7227,10 @@
     </row>
     <row r="272" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C272" s="2" t="b">
         <v>1</v>
@@ -7136,10 +7245,10 @@
     </row>
     <row r="273" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C273" s="2" t="b">
         <v>1</v>
@@ -7154,10 +7263,10 @@
     </row>
     <row r="274" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C274" s="2" t="b">
         <v>1</v>
@@ -7172,10 +7281,10 @@
     </row>
     <row r="275" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C275" s="2" t="b">
         <v>0</v>
@@ -7190,10 +7299,10 @@
     </row>
     <row r="276" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C276" s="2" t="b">
         <v>0</v>
@@ -7208,10 +7317,10 @@
     </row>
     <row r="277" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C277" s="2" t="b">
         <v>0</v>
@@ -7226,10 +7335,10 @@
     </row>
     <row r="278" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C278" s="2" t="b">
         <v>0</v>
@@ -7244,10 +7353,10 @@
     </row>
     <row r="279" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C279" s="2" t="b">
         <v>0</v>
@@ -7262,10 +7371,10 @@
     </row>
     <row r="280" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C280" s="2" t="b">
         <v>0</v>
@@ -7280,17 +7389,17 @@
     </row>
     <row r="281" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C281" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D281" s="2"/>
       <c r="E281" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F281" s="5"/>
       <c r="G281" s="2" t="str">
@@ -7300,17 +7409,17 @@
     </row>
     <row r="282" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C282" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D282" s="2"/>
       <c r="E282" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F282" s="5"/>
       <c r="G282" s="2" t="str">
@@ -7320,17 +7429,17 @@
     </row>
     <row r="283" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C283" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D283" s="2"/>
       <c r="E283" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F283" s="2"/>
       <c r="G283" s="2" t="str">
@@ -7340,10 +7449,10 @@
     </row>
     <row r="284" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C284" s="2" t="b">
         <v>0</v>
@@ -7358,10 +7467,10 @@
     </row>
     <row r="285" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C285" s="2" t="b">
         <v>0</v>
@@ -7376,10 +7485,10 @@
     </row>
     <row r="286" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C286" s="2" t="b">
         <v>1</v>
@@ -7394,10 +7503,10 @@
     </row>
     <row r="287" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C287" s="2" t="b">
         <v>1</v>
@@ -7412,10 +7521,10 @@
     </row>
     <row r="288" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C288" s="2" t="b">
         <v>1</v>
@@ -7430,10 +7539,10 @@
     </row>
     <row r="289" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C289" s="2" t="b">
         <v>1</v>
@@ -7448,10 +7557,10 @@
     </row>
     <row r="290" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C290" s="2" t="b">
         <v>1</v>
@@ -7466,10 +7575,10 @@
     </row>
     <row r="291" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C291" s="2" t="b">
         <v>0</v>
@@ -7484,10 +7593,10 @@
     </row>
     <row r="292" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C292" s="2" t="b">
         <v>0</v>
@@ -7502,10 +7611,10 @@
     </row>
     <row r="293" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C293" s="2" t="b">
         <v>0</v>
@@ -7520,10 +7629,10 @@
     </row>
     <row r="294" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C294" s="2" t="b">
         <v>0</v>
@@ -7538,10 +7647,10 @@
     </row>
     <row r="295" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C295" s="2" t="b">
         <v>0</v>
@@ -7558,10 +7667,10 @@
     </row>
     <row r="296" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C296" s="2" t="b">
         <v>0</v>
@@ -7576,10 +7685,10 @@
     </row>
     <row r="297" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C297" s="2" t="b">
         <v>0</v>
@@ -7594,10 +7703,10 @@
     </row>
     <row r="298" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C298" s="2" t="b">
         <v>0</v>
@@ -7612,10 +7721,10 @@
     </row>
     <row r="299" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C299" s="2" t="b">
         <v>0</v>
@@ -7630,10 +7739,10 @@
     </row>
     <row r="300" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C300" s="2" t="b">
         <v>0</v>
@@ -7648,10 +7757,10 @@
     </row>
     <row r="301" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C301" s="2" t="b">
         <v>0</v>
@@ -7666,10 +7775,10 @@
     </row>
     <row r="302" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C302" s="2" t="b">
         <v>0</v>
@@ -7684,10 +7793,10 @@
     </row>
     <row r="303" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C303" s="2" t="b">
         <v>0</v>
@@ -7702,16 +7811,16 @@
     </row>
     <row r="304" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C304" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D304" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B304" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C304" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D304" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="E304" s="2"/>
       <c r="F304" s="2"/>
@@ -7722,10 +7831,10 @@
     </row>
     <row r="305" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C305" s="2" t="b">
         <v>1</v>
@@ -7740,16 +7849,16 @@
     </row>
     <row r="306" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C306" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D306" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="C306" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D306" s="2" t="s">
-        <v>334</v>
       </c>
       <c r="E306" s="2"/>
       <c r="F306" s="2"/>
@@ -7760,17 +7869,17 @@
     </row>
     <row r="307" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C307" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D307" s="2"/>
       <c r="E307" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F307" s="2"/>
       <c r="G307" s="2" t="str">
@@ -7780,17 +7889,17 @@
     </row>
     <row r="308" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C308" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D308" s="2"/>
       <c r="E308" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F308" s="2"/>
       <c r="G308" s="2" t="str">
@@ -7800,17 +7909,17 @@
     </row>
     <row r="309" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C309" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D309" s="2"/>
       <c r="E309" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F309" s="2"/>
       <c r="G309" s="2" t="str">
@@ -7820,16 +7929,16 @@
     </row>
     <row r="310" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C310" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E310" s="2"/>
       <c r="F310" s="2"/>
@@ -7840,17 +7949,17 @@
     </row>
     <row r="311" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C311" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D311" s="2"/>
       <c r="E311" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F311" s="2"/>
       <c r="G311" s="2" t="str">
@@ -7860,10 +7969,10 @@
     </row>
     <row r="312" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C312" s="2" t="b">
         <v>0</v>
@@ -7878,30 +7987,30 @@
     </row>
     <row r="313" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C313" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D313" s="2"/>
       <c r="E313" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F313" s="2"/>
       <c r="G313" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Herbs &amp; Spices", category: "Condiments", avoid: false, measurement: "", notes: "Check for no onion or garlic in ingredients.", emoji: '' },</v>
+        <v>{ name: "Herbs &amp; Spices", category: "Condiments", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
       </c>
     </row>
     <row r="314" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C314" s="2" t="b">
         <v>0</v>
@@ -7916,10 +8025,10 @@
     </row>
     <row r="315" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C315" s="2" t="b">
         <v>0</v>
@@ -7934,10 +8043,10 @@
     </row>
     <row r="316" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C316" s="2" t="b">
         <v>0</v>
@@ -7952,10 +8061,10 @@
     </row>
     <row r="317" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C317" s="2" t="b">
         <v>0</v>
@@ -7970,10 +8079,10 @@
     </row>
     <row r="318" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C318" s="2" t="b">
         <v>0</v>
@@ -7988,10 +8097,10 @@
     </row>
     <row r="319" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C319" s="2" t="b">
         <v>0</v>
@@ -8006,10 +8115,10 @@
     </row>
     <row r="320" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C320" s="2" t="b">
         <v>0</v>
@@ -8024,10 +8133,10 @@
     </row>
     <row r="321" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C321" s="2" t="b">
         <v>0</v>
@@ -8042,10 +8151,10 @@
     </row>
     <row r="322" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C322" s="2" t="b">
         <v>0</v>
@@ -8060,10 +8169,10 @@
     </row>
     <row r="323" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C323" s="2" t="b">
         <v>0</v>
@@ -8078,10 +8187,10 @@
     </row>
     <row r="324" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C324" s="2" t="b">
         <v>0</v>
@@ -8096,10 +8205,10 @@
     </row>
     <row r="325" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C325" s="2" t="b">
         <v>0</v>
@@ -8114,10 +8223,10 @@
     </row>
     <row r="326" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C326" s="2" t="b">
         <v>0</v>
@@ -8132,10 +8241,10 @@
     </row>
     <row r="327" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C327" s="2" t="b">
         <v>0</v>
@@ -8150,17 +8259,17 @@
     </row>
     <row r="328" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C328" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D328" s="2"/>
       <c r="E328" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F328" s="2"/>
       <c r="G328" s="2" t="str">
@@ -8170,16 +8279,16 @@
     </row>
     <row r="329" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C329" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E329" s="2"/>
       <c r="F329" s="2"/>
@@ -8190,10 +8299,10 @@
     </row>
     <row r="330" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C330" s="2" t="b">
         <v>0</v>
@@ -8208,10 +8317,10 @@
     </row>
     <row r="331" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C331" s="2" t="b">
         <v>0</v>
@@ -8226,10 +8335,10 @@
     </row>
     <row r="332" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C332" s="2" t="b">
         <v>0</v>
@@ -8244,10 +8353,10 @@
     </row>
     <row r="333" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C333" s="2" t="b">
         <v>0</v>
@@ -8262,10 +8371,10 @@
     </row>
     <row r="334" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C334" s="2" t="b">
         <v>1</v>
@@ -8280,10 +8389,10 @@
     </row>
     <row r="335" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C335" s="2" t="b">
         <v>1</v>
@@ -8298,10 +8407,10 @@
     </row>
     <row r="336" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C336" s="2" t="b">
         <v>1</v>
@@ -8316,10 +8425,10 @@
     </row>
     <row r="337" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C337" s="2" t="b">
         <v>1</v>
@@ -8334,10 +8443,10 @@
     </row>
     <row r="338" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C338" s="2" t="b">
         <v>1</v>
@@ -8352,30 +8461,30 @@
     </row>
     <row r="339" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C339" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D339" s="2"/>
-      <c r="E339" s="2" t="s">
-        <v>447</v>
-      </c>
+      <c r="D339" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E339" s="2"/>
       <c r="F339" s="2"/>
       <c r="G339" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>{ name: "Hummus", category: "Condiments", avoid: true, measurement: "", notes: "&gt; 1 tablespoon", emoji: '' },</v>
+        <f>CONCATENATE("{ name: "&amp;CHAR(34),A339 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B339&amp;CHAR(34), ", ", "avoid: ", LOWER(C339), ", measurement: "&amp;CHAR(34), D339, CHAR(34), ", notes: ", CHAR(34), E339, CHAR(34), ", emoji: '", F339, "'", " },")</f>
+        <v>{ name: "Hummus", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C340" s="2" t="b">
         <v>1</v>
@@ -8390,10 +8499,10 @@
     </row>
     <row r="341" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C341" s="2" t="b">
         <v>1</v>
@@ -8408,150 +8517,150 @@
     </row>
     <row r="342" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C342" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D342" s="2"/>
-      <c r="E342" s="2" t="s">
-        <v>447</v>
-      </c>
+      <c r="D342" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E342" s="2"/>
       <c r="F342" s="2"/>
       <c r="G342" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Tahini", category: "Condiments", avoid: true, measurement: "", notes: "&gt; 1 tablespoon", emoji: '' },</v>
+        <v>{ name: "Tahini", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="343" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C343" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D343" s="2"/>
-      <c r="E343" s="2" t="s">
-        <v>374</v>
-      </c>
+      <c r="D343" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E343" s="2"/>
       <c r="F343" s="2"/>
       <c r="G343" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Cranberry Juice", category: "Drinks", avoid: false, measurement: "", notes: "1 cup", emoji: '' },</v>
+        <v>{ name: "Cranberry Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="344" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C344" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D344" s="2"/>
-      <c r="E344" s="2" t="s">
-        <v>374</v>
-      </c>
+      <c r="D344" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E344" s="2"/>
       <c r="F344" s="2"/>
       <c r="G344" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Tomato Juice", category: "Drinks", avoid: false, measurement: "", notes: "1 cup", emoji: '' },</v>
+        <v>{ name: "Tomato Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C345" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D345" s="2"/>
-      <c r="E345" s="2" t="s">
-        <v>374</v>
-      </c>
+      <c r="D345" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E345" s="2"/>
       <c r="F345" s="2"/>
       <c r="G345" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Lime Juice", category: "Drinks", avoid: false, measurement: "", notes: "1 cup", emoji: '' },</v>
+        <v>{ name: "Lime Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="346" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C346" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D346" s="2"/>
-      <c r="E346" s="2" t="s">
-        <v>374</v>
-      </c>
+      <c r="D346" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E346" s="2"/>
       <c r="F346" s="2"/>
       <c r="G346" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Lemon Juice", category: "Drinks", avoid: false, measurement: "", notes: "1 cup", emoji: '' },</v>
+        <v>{ name: "Lemon Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="347" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C347" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D347" s="2"/>
-      <c r="E347" s="2" t="s">
-        <v>374</v>
-      </c>
+      <c r="D347" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E347" s="2"/>
       <c r="F347" s="2"/>
       <c r="G347" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Spirulina Juice", category: "Drinks", avoid: false, measurement: "", notes: "1 cup", emoji: '' },</v>
+        <v>{ name: "Spirulina Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="348" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C348" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D348" s="2"/>
-      <c r="E348" s="5" t="s">
+      <c r="D348" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E348" s="5"/>
       <c r="F348" s="5"/>
       <c r="G348" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Orange Juice (Fresh)", category: "Drinks", avoid: false, measurement: "", notes: "½ cup", emoji: '' },</v>
+        <v>{ name: "Orange Juice (Fresh)", category: "Drinks", avoid: false, measurement: "½ cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="349" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C349" s="2" t="b">
         <v>0</v>
@@ -8566,10 +8675,10 @@
     </row>
     <row r="350" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C350" s="2" t="b">
         <v>0</v>
@@ -8584,10 +8693,10 @@
     </row>
     <row r="351" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C351" s="2" t="b">
         <v>0</v>
@@ -8602,10 +8711,10 @@
     </row>
     <row r="352" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C352" s="2" t="b">
         <v>0</v>
@@ -8620,10 +8729,10 @@
     </row>
     <row r="353" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C353" s="2" t="b">
         <v>0</v>
@@ -8638,10 +8747,10 @@
     </row>
     <row r="354" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C354" s="2" t="b">
         <v>0</v>
@@ -8656,10 +8765,10 @@
     </row>
     <row r="355" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C355" s="2" t="b">
         <v>0</v>
@@ -8674,10 +8783,10 @@
     </row>
     <row r="356" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C356" s="2" t="b">
         <v>0</v>
@@ -8692,10 +8801,10 @@
     </row>
     <row r="357" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C357" s="2" t="b">
         <v>0</v>
@@ -8710,10 +8819,10 @@
     </row>
     <row r="358" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C358" s="2" t="b">
         <v>0</v>
@@ -8728,10 +8837,10 @@
     </row>
     <row r="359" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C359" s="2" t="b">
         <v>0</v>
@@ -8746,10 +8855,10 @@
     </row>
     <row r="360" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C360" s="2" t="b">
         <v>0</v>
@@ -8764,10 +8873,10 @@
     </row>
     <row r="361" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C361" s="2" t="b">
         <v>0</v>
@@ -8782,30 +8891,30 @@
     </row>
     <row r="362" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C362" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D362" s="2"/>
-      <c r="E362" s="5" t="s">
-        <v>239</v>
-      </c>
+      <c r="D362" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E362" s="5"/>
       <c r="F362" s="5"/>
       <c r="G362" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Coconut Water", category: "Drinks", avoid: true, measurement: "", notes: "&gt; ½ cup", emoji: '' },</v>
+        <v>{ name: "Coconut Water", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="363" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C363" s="2" t="b">
         <v>1</v>
@@ -8820,10 +8929,10 @@
     </row>
     <row r="364" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C364" s="2" t="b">
         <v>1</v>
@@ -8838,10 +8947,10 @@
     </row>
     <row r="365" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C365" s="2" t="b">
         <v>1</v>
@@ -8856,30 +8965,30 @@
     </row>
     <row r="366" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C366" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D366" s="2"/>
-      <c r="E366" s="5" t="s">
-        <v>239</v>
-      </c>
+      <c r="D366" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E366" s="5"/>
       <c r="F366" s="5"/>
       <c r="G366" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Kombucha", category: "Drinks", avoid: true, measurement: "", notes: "&gt; ½ cup", emoji: '' },</v>
+        <v>{ name: "Kombucha", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '' },</v>
       </c>
     </row>
     <row r="367" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C367" s="2" t="b">
         <v>1</v>
@@ -8894,10 +9003,10 @@
     </row>
     <row r="368" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C368" s="2" t="b">
         <v>1</v>
@@ -8912,10 +9021,10 @@
     </row>
     <row r="369" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C369" s="2" t="b">
         <v>1</v>
@@ -8930,10 +9039,10 @@
     </row>
     <row r="370" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C370" s="2" t="b">
         <v>1</v>
@@ -8948,10 +9057,10 @@
     </row>
     <row r="371" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C371" s="2" t="b">
         <v>1</v>
@@ -8966,10 +9075,10 @@
     </row>
     <row r="372" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C372" s="2" t="b">
         <v>1</v>
@@ -8984,10 +9093,10 @@
     </row>
     <row r="373" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C373" s="2" t="b">
         <v>1</v>
@@ -9002,10 +9111,10 @@
     </row>
     <row r="374" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C374" s="2" t="b">
         <v>1</v>
@@ -9020,10 +9129,10 @@
     </row>
     <row r="375" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C375" s="2" t="b">
         <v>1</v>
@@ -9038,10 +9147,10 @@
     </row>
     <row r="376" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C376" s="2" t="b">
         <v>1</v>
@@ -9056,10 +9165,10 @@
     </row>
     <row r="377" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C377" s="2" t="b">
         <v>1</v>
@@ -9097,7 +9206,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Styling and data updates
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fodmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BB315E-FD67-4DA2-8D1F-ED5F082B2FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC6E90A-1536-4CEE-AF56-B6A6FDD9E2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="285" xr2:uid="{5144C98B-C405-4E2F-B3EA-D69079E9313A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="285" xr2:uid="{5144C98B-C405-4E2F-B3EA-D69079E9313A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="481">
   <si>
     <t>Name</t>
   </si>
@@ -1478,6 +1478,30 @@
   </si>
   <si>
     <t>🌷</t>
+  </si>
+  <si>
+    <t>🍞</t>
+  </si>
+  <si>
+    <t>🌾</t>
+  </si>
+  <si>
+    <t>🍫</t>
+  </si>
+  <si>
+    <t>🥣</t>
+  </si>
+  <si>
+    <t>🫧</t>
+  </si>
+  <si>
+    <t>🍝</t>
+  </si>
+  <si>
+    <t>🍚</t>
+  </si>
+  <si>
+    <t>🍜</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1913,8 @@
   <dimension ref="A1:G377"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G377"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F168" sqref="F168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4645,10 +4669,12 @@
         <v>16</v>
       </c>
       <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
+      <c r="F134" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="G134" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Bread", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '' },</v>
+        <v>{ name: "Bread", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4663,10 +4689,12 @@
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
+      <c r="F135" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G135" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Buckwheat", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Buckwheat", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4681,10 +4709,12 @@
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
+      <c r="F136" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G136" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Cacao Powder", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cacao Powder", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4701,10 +4731,12 @@
         <v>451</v>
       </c>
       <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
+      <c r="F137" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G137" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Carob", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "1 heaped teaspoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Carob", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "1 heaped teaspoon", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4719,10 +4751,12 @@
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
+      <c r="F138" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="G138" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Corn Flour", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Corn Flour", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌽' },</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4737,10 +4771,12 @@
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
+      <c r="F139" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="G139" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Corn Starch", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Corn Starch", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌽' },</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4755,10 +4791,12 @@
       </c>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
+      <c r="F140" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G140" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Fruit-Free Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fruit-Free Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4773,10 +4811,12 @@
       </c>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
+      <c r="F141" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G141" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "FODMAP Certified Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "FODMAP Certified Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4791,10 +4831,12 @@
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
+      <c r="F142" s="2" t="s">
+        <v>477</v>
+      </c>
       <c r="G142" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Guar Gum", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Guar Gum", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🫧' },</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4809,10 +4851,12 @@
       </c>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
+      <c r="F143" s="2" t="s">
+        <v>477</v>
+      </c>
       <c r="G143" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Xanthan Gum", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Xanthan Gum", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🫧' },</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4827,10 +4871,12 @@
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
+      <c r="F144" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G144" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Rolled Oats", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rolled Oats", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4845,10 +4891,12 @@
       </c>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
+      <c r="F145" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G145" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Fruit-Free Muesli", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fruit-Free Muesli", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4863,10 +4911,12 @@
       </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
-      <c r="F146" s="2"/>
+      <c r="F146" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="G146" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Corn Cous-Cous", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Corn Cous-Cous", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌽' },</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4883,10 +4933,12 @@
       <c r="E147" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="F147" s="2"/>
+      <c r="F147" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G147" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "No soy/legume flours.", emoji: '' },</v>
+        <v>{ name: "Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "No soy/legume flours.", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4901,10 +4953,12 @@
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
+      <c r="F148" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G148" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Polenta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Polenta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4919,10 +4973,12 @@
       </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
+      <c r="F149" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G149" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Quinoa", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Quinoa", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4937,10 +4993,12 @@
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
+      <c r="F150" s="2" t="s">
+        <v>479</v>
+      </c>
       <c r="G150" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Rice", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rice", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🍚' },</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4955,10 +5013,12 @@
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
+      <c r="F151" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G151" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Rice Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rice Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4973,10 +5033,12 @@
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
+      <c r="F152" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G152" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Konjac", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Konjac", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4991,10 +5053,12 @@
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
+      <c r="F153" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G153" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Tapioca Flour", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Tapioca Flour", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5009,10 +5073,12 @@
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
+      <c r="F154" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G154" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Teff", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Teff", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5029,10 +5095,12 @@
         <v>16</v>
       </c>
       <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
+      <c r="F155" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="G155" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "FODMAP Certified Bread", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '' },</v>
+        <v>{ name: "FODMAP Certified Bread", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5049,10 +5117,12 @@
         <v>178</v>
       </c>
       <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
+      <c r="F156" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G156" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Gnocchi", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "80% Potato", notes: "", emoji: '' },</v>
+        <v>{ name: "Gnocchi", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "80% Potato", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5069,10 +5139,12 @@
         <v>16</v>
       </c>
       <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
+      <c r="F157" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="G157" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Sourdough (Wheat/Spelt)", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '' },</v>
+        <v>{ name: "Sourdough (Wheat/Spelt)", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "2 slices", notes: "", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5089,10 +5161,12 @@
         <v>180</v>
       </c>
       <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
+      <c r="F158" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="G158" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Wheat Bread (Regular)", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "Up to 1 slice", notes: "", emoji: '' },</v>
+        <v>{ name: "Wheat Bread (Regular)", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "Up to 1 slice", notes: "", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5109,10 +5183,12 @@
         <v>84</v>
       </c>
       <c r="E159" s="5"/>
-      <c r="F159" s="5"/>
+      <c r="F159" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G159" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Wheat Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "Up to ½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Wheat Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: false, measurement: "Up to ½ cup", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5127,10 +5203,12 @@
       </c>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
+      <c r="F160" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G160" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Besan Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Besan Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5145,10 +5223,12 @@
       </c>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
+      <c r="F161" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G161" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Chickpea Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Chickpea Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5163,10 +5243,12 @@
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
+      <c r="F162" s="2" t="s">
+        <v>457</v>
+      </c>
       <c r="G162" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Coconut Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Coconut Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥥' },</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5181,10 +5263,12 @@
       </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
+      <c r="F163" s="2" t="s">
+        <v>429</v>
+      </c>
       <c r="G163" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Garbanzo Bean Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Garbanzo Bean Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5199,10 +5283,12 @@
       </c>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
+      <c r="F164" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G164" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Inulin", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Inulin", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5217,10 +5303,12 @@
       </c>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
-      <c r="F165" s="2"/>
+      <c r="F165" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G165" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Lupin", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lupin", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5235,10 +5323,12 @@
       </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
+      <c r="F166" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G166" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Lupin Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lupin Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5253,10 +5343,12 @@
       </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
+      <c r="F167" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G167" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Soy Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Soy Flour", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5271,10 +5363,12 @@
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
+      <c r="F168" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G168" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Muesli/Cereal with Honey", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Muesli/Cereal with Honey", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished adding emoji to data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\fodmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC6E90A-1536-4CEE-AF56-B6A6FDD9E2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D27C7-B0A3-4DD5-B909-C1507696C9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="285" xr2:uid="{5144C98B-C405-4E2F-B3EA-D69079E9313A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="285" xr2:uid="{5144C98B-C405-4E2F-B3EA-D69079E9313A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="532">
   <si>
     <t>Name</t>
   </si>
@@ -1502,6 +1502,159 @@
   </si>
   <si>
     <t>🍜</t>
+  </si>
+  <si>
+    <t>🧃</t>
+  </si>
+  <si>
+    <t>🍪</t>
+  </si>
+  <si>
+    <t>🎂</t>
+  </si>
+  <si>
+    <t>🍲</t>
+  </si>
+  <si>
+    <t>🧀</t>
+  </si>
+  <si>
+    <t>🧘🏻‍♀️</t>
+  </si>
+  <si>
+    <t>🥛</t>
+  </si>
+  <si>
+    <t>🍨</t>
+  </si>
+  <si>
+    <t>🍦</t>
+  </si>
+  <si>
+    <t>🍬</t>
+  </si>
+  <si>
+    <t>🌵</t>
+  </si>
+  <si>
+    <t>🥜</t>
+  </si>
+  <si>
+    <t>🧆</t>
+  </si>
+  <si>
+    <t>🧱</t>
+  </si>
+  <si>
+    <t>🍳</t>
+  </si>
+  <si>
+    <t>🍗</t>
+  </si>
+  <si>
+    <t>🐟</t>
+  </si>
+  <si>
+    <t>🥓</t>
+  </si>
+  <si>
+    <t>🍖</t>
+  </si>
+  <si>
+    <t>🌭</t>
+  </si>
+  <si>
+    <t>🥩</t>
+  </si>
+  <si>
+    <t>🥙</t>
+  </si>
+  <si>
+    <t>🍭</t>
+  </si>
+  <si>
+    <t>🍮</t>
+  </si>
+  <si>
+    <t>🥨</t>
+  </si>
+  <si>
+    <t>🍟</t>
+  </si>
+  <si>
+    <t>🍿</t>
+  </si>
+  <si>
+    <t>🍥</t>
+  </si>
+  <si>
+    <t>🍘</t>
+  </si>
+  <si>
+    <t>🧈</t>
+  </si>
+  <si>
+    <t>🌿</t>
+  </si>
+  <si>
+    <t>🥚</t>
+  </si>
+  <si>
+    <t>🫙</t>
+  </si>
+  <si>
+    <t>🦪</t>
+  </si>
+  <si>
+    <t>🦐</t>
+  </si>
+  <si>
+    <t>🟢</t>
+  </si>
+  <si>
+    <t>🪦</t>
+  </si>
+  <si>
+    <t>🍛</t>
+  </si>
+  <si>
+    <t>🍯</t>
+  </si>
+  <si>
+    <t>🧂</t>
+  </si>
+  <si>
+    <t>🥤</t>
+  </si>
+  <si>
+    <t>☕</t>
+  </si>
+  <si>
+    <t>🍵</t>
+  </si>
+  <si>
+    <t>🫖</t>
+  </si>
+  <si>
+    <t>🍺</t>
+  </si>
+  <si>
+    <t>🥃</t>
+  </si>
+  <si>
+    <t>🍶</t>
+  </si>
+  <si>
+    <t>🍾</t>
+  </si>
+  <si>
+    <t>🍷</t>
+  </si>
+  <si>
+    <t>🍹</t>
+  </si>
+  <si>
+    <t>🧋</t>
   </si>
 </sst>
 </file>
@@ -1913,8 +2066,8 @@
   <dimension ref="A1:G377"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F168" sqref="F168"/>
+      <pane ySplit="1" topLeftCell="A363" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F377" sqref="F377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5383,10 +5536,12 @@
       </c>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
-      <c r="F169" s="2"/>
+      <c r="F169" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G169" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Muesli/Cereal with Dried Fruit", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Muesli/Cereal with Dried Fruit", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5401,10 +5556,12 @@
       </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
+      <c r="F170" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G170" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Muesli/Cereal with Fructose", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Muesli/Cereal with Fructose", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5419,10 +5576,12 @@
       </c>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
-      <c r="F171" s="2"/>
+      <c r="F171" s="2" t="s">
+        <v>481</v>
+      </c>
       <c r="G171" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Fruit Juice Concentrate", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fruit Juice Concentrate", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🧃' },</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5437,10 +5596,12 @@
       </c>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
-      <c r="F172" s="2"/>
+      <c r="F172" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G172" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Pasta (Chickpea Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pasta (Chickpea Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5455,10 +5616,12 @@
       </c>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
-      <c r="F173" s="2"/>
+      <c r="F173" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G173" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Pasta (Legume Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pasta (Legume Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5473,10 +5636,12 @@
       </c>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
+      <c r="F174" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G174" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Pasta (Soy Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pasta (Soy Flour)", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5491,10 +5656,12 @@
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
-      <c r="F175" s="2"/>
+      <c r="F175" s="2" t="s">
+        <v>479</v>
+      </c>
       <c r="G175" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Cauliflower Rice", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cauliflower Rice", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍚' },</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5509,10 +5676,12 @@
       </c>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
-      <c r="F176" s="2"/>
+      <c r="F176" s="2" t="s">
+        <v>473</v>
+      </c>
       <c r="G176" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Regular Breads", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Breads", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5527,10 +5696,12 @@
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
-      <c r="F177" s="2"/>
+      <c r="F177" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="G177" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Regular Biscuits", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Biscuits", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍪' },</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5545,10 +5716,12 @@
       </c>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
-      <c r="F178" s="2"/>
+      <c r="F178" s="2" t="s">
+        <v>483</v>
+      </c>
       <c r="G178" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Regular Cakes", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Cakes", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🎂' },</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5563,10 +5736,12 @@
       </c>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
-      <c r="F179" s="2"/>
+      <c r="F179" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G179" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Barley", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Barley", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5581,10 +5756,12 @@
       </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
-      <c r="F180" s="2"/>
+      <c r="F180" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G180" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Cous-Cous", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cous-Cous", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5599,10 +5776,12 @@
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
-      <c r="F181" s="2"/>
+      <c r="F181" s="2" t="s">
+        <v>474</v>
+      </c>
       <c r="G181" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Rye", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rye", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🌾' },</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5617,10 +5796,12 @@
       </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
-      <c r="F182" s="2"/>
+      <c r="F182" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G182" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Wheat-based Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Wheat-based Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5635,10 +5816,12 @@
       </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
-      <c r="F183" s="2"/>
+      <c r="F183" s="2" t="s">
+        <v>476</v>
+      </c>
       <c r="G183" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Bran-based Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Bran-based Cereals", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🥣' },</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5653,10 +5836,12 @@
       </c>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
-      <c r="F184" s="2"/>
+      <c r="F184" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G184" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Wheat Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Wheat Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5671,10 +5856,12 @@
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
-      <c r="F185" s="2"/>
+      <c r="F185" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G185" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Semolina Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Semolina Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5689,10 +5876,12 @@
       </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
-      <c r="F186" s="2"/>
+      <c r="F186" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G186" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Spelt Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Spelt Pasta", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5707,10 +5896,12 @@
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
-      <c r="F187" s="2"/>
+      <c r="F187" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G187" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Egg Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Egg Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5725,10 +5916,12 @@
       </c>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
-      <c r="F188" s="2"/>
+      <c r="F188" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G188" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Udon Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Udon Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5743,10 +5936,12 @@
       </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
-      <c r="F189" s="2"/>
+      <c r="F189" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G189" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Ramen", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Ramen", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5761,10 +5956,12 @@
       </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
-      <c r="F190" s="2"/>
+      <c r="F190" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G190" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Instant Wheat Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Instant Wheat Noodles", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5779,10 +5976,12 @@
       </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
-      <c r="F191" s="2"/>
+      <c r="F191" s="2" t="s">
+        <v>484</v>
+      </c>
       <c r="G191" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Noodle Soups", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Noodle Soups", category: "Gluten Free Cereals &amp; Grain", avoid: true, measurement: "", notes: "", emoji: '🍲' },</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5797,10 +5996,12 @@
       </c>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
-      <c r="F192" s="2"/>
+      <c r="F192" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="G192" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Cheese (Set/Firm)", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cheese (Set/Firm)", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '🧀' },</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5817,10 +6018,12 @@
         <v>448</v>
       </c>
       <c r="E193" s="2"/>
-      <c r="F193" s="2"/>
+      <c r="F193" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="G193" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Greek (Strained) Yoghurt", category: "Milk Products", avoid: false, measurement: "2 to 3 tablespoons", notes: "", emoji: '' },</v>
+        <v>{ name: "Greek (Strained) Yoghurt", category: "Milk Products", avoid: false, measurement: "2 to 3 tablespoons", notes: "", emoji: '🧘🏻‍♀️' },</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5835,10 +6038,12 @@
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
-      <c r="F194" s="2"/>
+      <c r="F194" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G194" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>{ name: "Lactose-Free Cow's Milk", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lactose-Free Cow's Milk", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5853,10 +6058,12 @@
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
-      <c r="F195" s="2"/>
+      <c r="F195" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G195" s="2" t="str">
         <f t="shared" ref="G195:G258" si="3">CONCATENATE("{ name: "&amp;CHAR(34),A195 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B195&amp;CHAR(34), ", ", "avoid: ", LOWER(C195), ", measurement: "&amp;CHAR(34), D195, CHAR(34), ", notes: ", CHAR(34), E195, CHAR(34), ", emoji: '", F195, "'", " },")</f>
-        <v>{ name: "Lactose-Free Cow's Milk Cream", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lactose-Free Cow's Milk Cream", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5871,10 +6078,12 @@
       </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
-      <c r="F196" s="2"/>
+      <c r="F196" s="2" t="s">
+        <v>488</v>
+      </c>
       <c r="G196" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Lactose-Free Cow's Milk Ice Cream", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lactose-Free Cow's Milk Ice Cream", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '🍨' },</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5889,10 +6098,12 @@
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
-      <c r="F197" s="2"/>
+      <c r="F197" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="G197" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Lactose-Free Cow's Milk Yoghurt", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Lactose-Free Cow's Milk Yoghurt", category: "Milk Products", avoid: false, measurement: "", notes: "", emoji: '🧘🏻‍♀️' },</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5909,10 +6120,12 @@
         <v>449</v>
       </c>
       <c r="E198" s="2"/>
-      <c r="F198" s="2"/>
+      <c r="F198" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="G198" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Ricotta", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '' },</v>
+        <v>{ name: "Ricotta", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '🧀' },</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5929,10 +6142,12 @@
         <v>449</v>
       </c>
       <c r="E199" s="2"/>
-      <c r="F199" s="2"/>
+      <c r="F199" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="G199" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Cream Cheese", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '' },</v>
+        <v>{ name: "Cream Cheese", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '🧀' },</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5949,10 +6164,12 @@
         <v>449</v>
       </c>
       <c r="E200" s="2"/>
-      <c r="F200" s="2"/>
+      <c r="F200" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G200" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Sour Cream", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '' },</v>
+        <v>{ name: "Sour Cream", category: "Milk Products", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5967,10 +6184,12 @@
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
-      <c r="F201" s="2"/>
+      <c r="F201" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G201" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Cow's Milk", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cow's Milk", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5985,10 +6204,12 @@
       </c>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
-      <c r="F202" s="2"/>
+      <c r="F202" s="2" t="s">
+        <v>489</v>
+      </c>
       <c r="G202" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Regular Ice Cream", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Ice Cream", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '🍦' },</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6003,10 +6224,12 @@
       </c>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
-      <c r="F203" s="2"/>
+      <c r="F203" s="2" t="s">
+        <v>486</v>
+      </c>
       <c r="G203" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Regular Yoghurt", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Yoghurt", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '🧘🏻‍♀️' },</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6021,10 +6244,12 @@
       </c>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
-      <c r="F204" s="2"/>
+      <c r="F204" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G204" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Regular Custard", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Regular Custard", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6039,10 +6264,12 @@
       </c>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
-      <c r="F205" s="2"/>
+      <c r="F205" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G205" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Milk Kefir", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Milk Kefir", category: "Milk Products", avoid: true, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="206" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6057,10 +6284,12 @@
       </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
-      <c r="F206" s="2"/>
+      <c r="F206" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G206" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Almond Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Almond Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="207" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6075,10 +6304,12 @@
       </c>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
-      <c r="F207" s="2"/>
+      <c r="F207" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G207" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Rice Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rice Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6093,10 +6324,12 @@
       </c>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
-      <c r="F208" s="2"/>
+      <c r="F208" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G208" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Quinoa Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Quinoa Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="209" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6111,10 +6344,12 @@
       </c>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
-      <c r="F209" s="2"/>
+      <c r="F209" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G209" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Hemp Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Hemp Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6131,10 +6366,12 @@
         <v>10</v>
       </c>
       <c r="E210" s="5"/>
-      <c r="F210" s="5"/>
+      <c r="F210" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="G210" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Coconut Milk (Tinned)", category: "Milk Alternatives", avoid: false, measurement: "½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Coconut Milk (Tinned)", category: "Milk Alternatives", avoid: false, measurement: "½ cup", notes: "", emoji: '🥥' },</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6151,10 +6388,12 @@
         <v>10</v>
       </c>
       <c r="E211" s="5"/>
-      <c r="F211" s="5"/>
+      <c r="F211" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="G211" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Coconut Cream", category: "Milk Alternatives", avoid: false, measurement: "½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Coconut Cream", category: "Milk Alternatives", avoid: false, measurement: "½ cup", notes: "", emoji: '🥥' },</v>
       </c>
     </row>
     <row r="212" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6169,10 +6408,12 @@
       </c>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
-      <c r="F212" s="2"/>
+      <c r="F212" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G212" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Pea Protein Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pea Protein Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6189,10 +6430,12 @@
       <c r="E213" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="F213" s="2"/>
+      <c r="F213" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G213" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Soy Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "Must be made from soy protein.", emoji: '' },</v>
+        <v>{ name: "Soy Milk", category: "Milk Alternatives", avoid: false, measurement: "", notes: "Must be made from soy protein.", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6209,10 +6452,12 @@
       <c r="E214" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F214" s="2"/>
+      <c r="F214" s="2" t="s">
+        <v>485</v>
+      </c>
       <c r="G214" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Soy Cheese", category: "Milk Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Soy Cheese", category: "Milk Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '🧀' },</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6229,10 +6474,12 @@
         <v>238</v>
       </c>
       <c r="E215" s="5"/>
-      <c r="F215" s="5"/>
+      <c r="F215" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G215" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Oat Milk", category: "Milk Alternatives", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Oat Milk", category: "Milk Alternatives", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="216" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6249,10 +6496,12 @@
       <c r="E216" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="F216" s="2"/>
+      <c r="F216" s="2" t="s">
+        <v>487</v>
+      </c>
       <c r="G216" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Soy Milk", category: "Milk Alternatives", avoid: true, measurement: "", notes: "Must be made from whole soy beans.", emoji: '' },</v>
+        <v>{ name: "Soy Milk", category: "Milk Alternatives", avoid: true, measurement: "", notes: "Must be made from whole soy beans.", emoji: '🥛' },</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6269,10 +6518,12 @@
         <v>444</v>
       </c>
       <c r="E217" s="2"/>
-      <c r="F217" s="2"/>
+      <c r="F217" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G217" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "White Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "White Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6289,10 +6540,12 @@
         <v>444</v>
       </c>
       <c r="E218" s="2"/>
-      <c r="F218" s="2"/>
+      <c r="F218" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G218" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Castor Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Castor Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6309,10 +6562,12 @@
         <v>444</v>
       </c>
       <c r="E219" s="2"/>
-      <c r="F219" s="2"/>
+      <c r="F219" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G219" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Icing Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Icing Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6329,10 +6584,12 @@
         <v>444</v>
       </c>
       <c r="E220" s="2"/>
-      <c r="F220" s="2"/>
+      <c r="F220" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G220" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Brown Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Brown Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6349,10 +6606,12 @@
         <v>444</v>
       </c>
       <c r="E221" s="2"/>
-      <c r="F221" s="2"/>
+      <c r="F221" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G221" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Coconut Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Coconut Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="222" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6369,10 +6628,12 @@
         <v>444</v>
       </c>
       <c r="E222" s="2"/>
-      <c r="F222" s="2"/>
+      <c r="F222" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G222" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Powdered Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Powdered Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="223" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6389,10 +6650,12 @@
         <v>444</v>
       </c>
       <c r="E223" s="2"/>
-      <c r="F223" s="2"/>
+      <c r="F223" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G223" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Glucose", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Glucose", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6409,10 +6672,12 @@
         <v>444</v>
       </c>
       <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
+      <c r="F224" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G224" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Glucose Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Glucose Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="225" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6429,10 +6694,12 @@
         <v>444</v>
       </c>
       <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
+      <c r="F225" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G225" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Dextrose", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Dextrose", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="226" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6449,10 +6716,12 @@
         <v>452</v>
       </c>
       <c r="E226" s="5"/>
-      <c r="F226" s="5"/>
+      <c r="F226" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G226" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Golden Syrup", category: "Sweeteners", avoid: false, measurement: "½ tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Golden Syrup", category: "Sweeteners", avoid: false, measurement: "½ tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6469,10 +6738,12 @@
         <v>444</v>
       </c>
       <c r="E227" s="2"/>
-      <c r="F227" s="2"/>
+      <c r="F227" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G227" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Invert Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Invert Sugar", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6489,10 +6760,12 @@
         <v>444</v>
       </c>
       <c r="E228" s="2"/>
-      <c r="F228" s="2"/>
+      <c r="F228" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G228" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Maple Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Maple Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6509,10 +6782,12 @@
         <v>452</v>
       </c>
       <c r="E229" s="5"/>
-      <c r="F229" s="5"/>
+      <c r="F229" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G229" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Molasses", category: "Sweeteners", avoid: false, measurement: "½ tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Molasses", category: "Sweeteners", avoid: false, measurement: "½ tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6529,10 +6804,12 @@
         <v>444</v>
       </c>
       <c r="E230" s="2"/>
-      <c r="F230" s="2"/>
+      <c r="F230" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G230" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Rice Malt Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Rice Malt Syrup", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6549,10 +6826,12 @@
         <v>444</v>
       </c>
       <c r="E231" s="2"/>
-      <c r="F231" s="2"/>
+      <c r="F231" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G231" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Stevia", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Stevia", category: "Sweeteners", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="232" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6567,10 +6846,12 @@
       </c>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
-      <c r="F232" s="2"/>
+      <c r="F232" s="2" t="s">
+        <v>491</v>
+      </c>
       <c r="G232" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Agave", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Agave", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🌵' },</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6585,10 +6866,12 @@
       </c>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
-      <c r="F233" s="2"/>
+      <c r="F233" s="2" t="s">
+        <v>440</v>
+      </c>
       <c r="G233" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Honeydew", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Honeydew", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍈' },</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6603,10 +6886,12 @@
       </c>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
-      <c r="F234" s="2"/>
+      <c r="F234" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G234" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Isomalt", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Isomalt", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6621,10 +6906,12 @@
       </c>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
-      <c r="F235" s="2"/>
+      <c r="F235" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G235" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Mannitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mannitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="236" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6639,10 +6926,12 @@
       </c>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
-      <c r="F236" s="2"/>
+      <c r="F236" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G236" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Maltilol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Maltilol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6657,10 +6946,12 @@
       </c>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
-      <c r="F237" s="2"/>
+      <c r="F237" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G237" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Sorbitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Sorbitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="238" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6675,10 +6966,12 @@
       </c>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
-      <c r="F238" s="2"/>
+      <c r="F238" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G238" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Treacle", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Treacle", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="239" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6693,10 +6986,12 @@
       </c>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
-      <c r="F239" s="2"/>
+      <c r="F239" s="2" t="s">
+        <v>490</v>
+      </c>
       <c r="G239" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Xylitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Xylitol", category: "Sweeteners", avoid: true, measurement: "", notes: "", emoji: '🍬' },</v>
       </c>
     </row>
     <row r="240" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6713,10 +7008,12 @@
         <v>263</v>
       </c>
       <c r="E240" s="2"/>
-      <c r="F240" s="2"/>
+      <c r="F240" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G240" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Almonds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Almonds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="241" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6733,10 +7030,12 @@
         <v>263</v>
       </c>
       <c r="E241" s="2"/>
-      <c r="F241" s="2"/>
+      <c r="F241" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G241" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Brazil Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Brazil Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6753,10 +7052,12 @@
         <v>263</v>
       </c>
       <c r="E242" s="2"/>
-      <c r="F242" s="2"/>
+      <c r="F242" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G242" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Hazelnuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Hazelnuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6773,10 +7074,12 @@
         <v>263</v>
       </c>
       <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
+      <c r="F243" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G243" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Mixed Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Mixed Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="244" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6793,10 +7096,12 @@
         <v>263</v>
       </c>
       <c r="E244" s="2"/>
-      <c r="F244" s="2"/>
+      <c r="F244" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G244" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Peanuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Peanuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="245" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6813,10 +7118,12 @@
         <v>263</v>
       </c>
       <c r="E245" s="2"/>
-      <c r="F245" s="2"/>
+      <c r="F245" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G245" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Pecans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Pecans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6833,10 +7140,12 @@
         <v>263</v>
       </c>
       <c r="E246" s="2"/>
-      <c r="F246" s="2"/>
+      <c r="F246" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G246" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Pine Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Pine Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6853,10 +7162,12 @@
         <v>263</v>
       </c>
       <c r="E247" s="2"/>
-      <c r="F247" s="2"/>
+      <c r="F247" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G247" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Walnuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Walnuts", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="248" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6873,10 +7184,12 @@
         <v>263</v>
       </c>
       <c r="E248" s="2"/>
-      <c r="F248" s="2"/>
+      <c r="F248" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G248" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Sesame Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Sesame Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6893,10 +7206,12 @@
         <v>263</v>
       </c>
       <c r="E249" s="2"/>
-      <c r="F249" s="2"/>
+      <c r="F249" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G249" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Sunflower Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Sunflower Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="250" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6913,10 +7228,12 @@
         <v>263</v>
       </c>
       <c r="E250" s="2"/>
-      <c r="F250" s="2"/>
+      <c r="F250" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G250" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Linseeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Linseeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="251" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6933,10 +7250,12 @@
         <v>263</v>
       </c>
       <c r="E251" s="2"/>
-      <c r="F251" s="2"/>
+      <c r="F251" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G251" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Poppy Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Poppy Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="252" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6953,10 +7272,12 @@
         <v>263</v>
       </c>
       <c r="E252" s="2"/>
-      <c r="F252" s="2"/>
+      <c r="F252" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G252" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Pepitas", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '' },</v>
+        <v>{ name: "Pepitas", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 handful", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="253" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6973,10 +7294,12 @@
         <v>29</v>
       </c>
       <c r="E253" s="5"/>
-      <c r="F253" s="5"/>
+      <c r="F253" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G253" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Canned Butter Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Canned Butter Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="254" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6993,10 +7316,12 @@
         <v>29</v>
       </c>
       <c r="E254" s="5"/>
-      <c r="F254" s="5"/>
+      <c r="F254" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G254" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Canned Chick Peas", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Canned Chick Peas", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="255" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7013,10 +7338,12 @@
         <v>29</v>
       </c>
       <c r="E255" s="5"/>
-      <c r="F255" s="5"/>
+      <c r="F255" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G255" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Canned Lentils", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Canned Lentils", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="256" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7033,10 +7360,12 @@
         <v>29</v>
       </c>
       <c r="E256" s="5"/>
-      <c r="F256" s="5"/>
+      <c r="F256" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G256" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Lima Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Lima Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="257" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7053,10 +7382,12 @@
         <v>444</v>
       </c>
       <c r="E257" s="5"/>
-      <c r="F257" s="5"/>
+      <c r="F257" s="2" t="s">
+        <v>419</v>
+      </c>
       <c r="G257" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Chia Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Chia Seeds", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🌱' },</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7075,10 +7406,12 @@
       <c r="E258" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F258" s="2"/>
+      <c r="F258" s="2" t="s">
+        <v>493</v>
+      </c>
       <c r="G258" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>{ name: "Quorn", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Quorn", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "No onion or garlic.", emoji: '🧆' },</v>
       </c>
     </row>
     <row r="259" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7097,10 +7430,12 @@
       <c r="E259" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F259" s="2"/>
+      <c r="F259" s="2" t="s">
+        <v>493</v>
+      </c>
       <c r="G259" s="2" t="str">
         <f t="shared" ref="G259:G322" si="4">CONCATENATE("{ name: "&amp;CHAR(34),A259 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B259&amp;CHAR(34), ", ", "avoid: ", LOWER(C259), ", measurement: "&amp;CHAR(34), D259, CHAR(34), ", notes: ", CHAR(34), E259, CHAR(34), ", emoji: '", F259, "'", " },")</f>
-        <v>{ name: "Tempeh", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Tempeh", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "¼ cup", notes: "No onion or garlic.", emoji: '🧆' },</v>
       </c>
     </row>
     <row r="260" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7115,10 +7450,12 @@
       </c>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
-      <c r="F260" s="2"/>
+      <c r="F260" s="2" t="s">
+        <v>494</v>
+      </c>
       <c r="G260" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Tofu (Firm)", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Tofu (Firm)", category: "Nuts, Seeds, &amp; Legumes", avoid: false, measurement: "", notes: "", emoji: '🧱' },</v>
       </c>
     </row>
     <row r="261" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7133,10 +7470,12 @@
       </c>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
-      <c r="F261" s="2"/>
+      <c r="F261" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G261" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Cashews", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cashews", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="262" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7151,10 +7490,12 @@
       </c>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
-      <c r="F262" s="2"/>
+      <c r="F262" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G262" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Pistachio Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pistachio Nuts", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="263" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7169,10 +7510,12 @@
       </c>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
-      <c r="F263" s="2"/>
+      <c r="F263" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G263" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Baked Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Baked Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="264" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7187,10 +7530,12 @@
       </c>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
-      <c r="F264" s="2"/>
+      <c r="F264" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G264" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Black Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Black Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="265" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7205,10 +7550,12 @@
       </c>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
-      <c r="F265" s="2"/>
+      <c r="F265" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G265" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Borlotti Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Borlotti Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="266" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7223,10 +7570,12 @@
       </c>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
-      <c r="F266" s="2"/>
+      <c r="F266" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G266" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Broad Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Broad Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="267" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7241,10 +7590,12 @@
       </c>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
-      <c r="F267" s="2"/>
+      <c r="F267" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G267" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Cannellini Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cannellini Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="268" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7259,10 +7610,12 @@
       </c>
       <c r="D268" s="2"/>
       <c r="E268" s="2"/>
-      <c r="F268" s="2"/>
+      <c r="F268" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G268" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Fava Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fava Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="269" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7277,10 +7630,12 @@
       </c>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
-      <c r="F269" s="2"/>
+      <c r="F269" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G269" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Four Bean Mix", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Four Bean Mix", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="270" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7295,10 +7650,12 @@
       </c>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
-      <c r="F270" s="2"/>
+      <c r="F270" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G270" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Garbanzo Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Garbanzo Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="271" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7313,10 +7670,12 @@
       </c>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
-      <c r="F271" s="2"/>
+      <c r="F271" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G271" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Haricot Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Haricot Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="272" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7331,10 +7690,12 @@
       </c>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
-      <c r="F272" s="2"/>
+      <c r="F272" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G272" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Navy Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Navy Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="273" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7349,10 +7710,12 @@
       </c>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
-      <c r="F273" s="2"/>
+      <c r="F273" s="5" t="s">
+        <v>429</v>
+      </c>
       <c r="G273" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Soy Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Soy Beans", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🫘' },</v>
       </c>
     </row>
     <row r="274" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7367,10 +7730,12 @@
       </c>
       <c r="D274" s="2"/>
       <c r="E274" s="2"/>
-      <c r="F274" s="2"/>
+      <c r="F274" s="2" t="s">
+        <v>489</v>
+      </c>
       <c r="G274" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Tofu (Silken)", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Tofu (Silken)", category: "Nuts, Seeds, &amp; Legumes", avoid: true, measurement: "", notes: "", emoji: '🍦' },</v>
       </c>
     </row>
     <row r="275" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7385,10 +7750,12 @@
       </c>
       <c r="D275" s="2"/>
       <c r="E275" s="2"/>
-      <c r="F275" s="2"/>
+      <c r="F275" s="2" t="s">
+        <v>495</v>
+      </c>
       <c r="G275" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Eggs", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Eggs", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🍳' },</v>
       </c>
     </row>
     <row r="276" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7403,10 +7770,12 @@
       </c>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
-      <c r="F276" s="2"/>
+      <c r="F276" s="2" t="s">
+        <v>496</v>
+      </c>
       <c r="G276" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Chicken (Fresh cuts/Minced/Ground)", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Chicken (Fresh cuts/Minced/Ground)", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🍗' },</v>
       </c>
     </row>
     <row r="277" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7421,10 +7790,12 @@
       </c>
       <c r="D277" s="2"/>
       <c r="E277" s="2"/>
-      <c r="F277" s="2"/>
+      <c r="F277" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G277" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Fish (Fresh cuts/Minced/Ground)", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fish (Fresh cuts/Minced/Ground)", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="278" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7439,10 +7810,12 @@
       </c>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
-      <c r="F278" s="2"/>
+      <c r="F278" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G278" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Tinned Fish", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Tinned Fish", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="279" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7457,10 +7830,12 @@
       </c>
       <c r="D279" s="2"/>
       <c r="E279" s="2"/>
-      <c r="F279" s="2"/>
+      <c r="F279" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G279" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Plain Grilled Fish", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Plain Grilled Fish", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="280" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7475,10 +7850,12 @@
       </c>
       <c r="D280" s="2"/>
       <c r="E280" s="2"/>
-      <c r="F280" s="2"/>
+      <c r="F280" s="2" t="s">
+        <v>498</v>
+      </c>
       <c r="G280" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most Bacon/Ham/Salami", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most Bacon/Ham/Salami", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🥓' },</v>
       </c>
     </row>
     <row r="281" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7495,10 +7872,12 @@
       <c r="E281" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="F281" s="5"/>
+      <c r="F281" s="5" t="s">
+        <v>499</v>
+      </c>
       <c r="G281" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Meat Products", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Meat Products", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '🍖' },</v>
       </c>
     </row>
     <row r="282" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7515,10 +7894,12 @@
       <c r="E282" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="F282" s="5"/>
+      <c r="F282" s="5" t="s">
+        <v>473</v>
+      </c>
       <c r="G282" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "GF Battered/Bread-Crumbed Products", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "GF Battered/Bread-Crumbed Products", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '🍞' },</v>
       </c>
     </row>
     <row r="283" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7535,10 +7916,12 @@
       <c r="E283" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="F283" s="2"/>
+      <c r="F283" s="2" t="s">
+        <v>494</v>
+      </c>
       <c r="G283" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Firm Tofu", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "Check flavours and spices in the ingredients.", emoji: '' },</v>
+        <v>{ name: "Firm Tofu", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "Check flavours and spices in the ingredients.", emoji: '🧱' },</v>
       </c>
     </row>
     <row r="284" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7553,10 +7936,12 @@
       </c>
       <c r="D284" s="2"/>
       <c r="E284" s="2"/>
-      <c r="F284" s="2"/>
+      <c r="F284" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G284" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Smoked Trout", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Smoked Trout", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="285" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7571,10 +7956,12 @@
       </c>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
-      <c r="F285" s="2"/>
+      <c r="F285" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G285" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Smoked Salmon", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Smoked Salmon", category: "Meat &amp; Alternatives", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="286" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7589,10 +7976,12 @@
       </c>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
-      <c r="F286" s="2"/>
+      <c r="F286" s="2" t="s">
+        <v>500</v>
+      </c>
       <c r="G286" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Sausages containing Onion/Garlic Powder", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Sausages containing Onion/Garlic Powder", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '🌭' },</v>
       </c>
     </row>
     <row r="287" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7607,10 +7996,12 @@
       </c>
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
-      <c r="F287" s="2"/>
+      <c r="F287" s="2" t="s">
+        <v>501</v>
+      </c>
       <c r="G287" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most crumbed or battered meat", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most crumbed or battered meat", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '🥩' },</v>
       </c>
     </row>
     <row r="288" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7625,10 +8016,12 @@
       </c>
       <c r="D288" s="2"/>
       <c r="E288" s="2"/>
-      <c r="F288" s="2"/>
+      <c r="F288" s="2" t="s">
+        <v>496</v>
+      </c>
       <c r="G288" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most crumbed or battered chicken", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most crumbed or battered chicken", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '🍗' },</v>
       </c>
     </row>
     <row r="289" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7643,10 +8036,12 @@
       </c>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
-      <c r="F289" s="2"/>
+      <c r="F289" s="2" t="s">
+        <v>497</v>
+      </c>
       <c r="G289" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most crumbed or battered fish", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most crumbed or battered fish", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="290" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7661,10 +8056,12 @@
       </c>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
-      <c r="F290" s="2"/>
+      <c r="F290" s="2" t="s">
+        <v>502</v>
+      </c>
       <c r="G290" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most Vegetarian Burgers/Falafel", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most Vegetarian Burgers/Falafel", category: "Meat &amp; Alternatives", avoid: true, measurement: "", notes: "", emoji: '🥙' },</v>
       </c>
     </row>
     <row r="291" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7679,10 +8076,12 @@
       </c>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
-      <c r="F291" s="2"/>
+      <c r="F291" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G291" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Dark Chocolate", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Dark Chocolate", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="292" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7697,10 +8096,12 @@
       </c>
       <c r="D292" s="2"/>
       <c r="E292" s="2"/>
-      <c r="F292" s="2"/>
+      <c r="F292" s="2" t="s">
+        <v>503</v>
+      </c>
       <c r="G292" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Most Jelly Beans/Lollies", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Most Jelly Beans/Lollies", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍭' },</v>
       </c>
     </row>
     <row r="293" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7715,10 +8116,12 @@
       </c>
       <c r="D293" s="2"/>
       <c r="E293" s="2"/>
-      <c r="F293" s="2"/>
+      <c r="F293" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G293" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Fruit-Free Muesli Bars", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fruit-Free Muesli Bars", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="294" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7733,10 +8136,12 @@
       </c>
       <c r="D294" s="2"/>
       <c r="E294" s="2"/>
-      <c r="F294" s="2"/>
+      <c r="F294" s="2" t="s">
+        <v>504</v>
+      </c>
       <c r="G294" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Jelly", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Jelly", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍮' },</v>
       </c>
     </row>
     <row r="295" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7753,10 +8158,12 @@
         <v>10</v>
       </c>
       <c r="E295" s="5"/>
-      <c r="F295" s="5"/>
+      <c r="F295" s="5" t="s">
+        <v>505</v>
+      </c>
       <c r="G295" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Pretzels (Regular)", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Pretzels (Regular)", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "½ cup", notes: "", emoji: '🥨' },</v>
       </c>
     </row>
     <row r="296" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7771,10 +8178,12 @@
       </c>
       <c r="D296" s="2"/>
       <c r="E296" s="2"/>
-      <c r="F296" s="2"/>
+      <c r="F296" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="G296" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Plain Hot Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Plain Hot Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍟' },</v>
       </c>
     </row>
     <row r="297" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7789,10 +8198,12 @@
       </c>
       <c r="D297" s="2"/>
       <c r="E297" s="2"/>
-      <c r="F297" s="2"/>
+      <c r="F297" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="G297" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Plain Salted Potato Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Plain Salted Potato Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍟' },</v>
       </c>
     </row>
     <row r="298" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7807,10 +8218,12 @@
       </c>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
-      <c r="F298" s="2"/>
+      <c r="F298" s="2" t="s">
+        <v>507</v>
+      </c>
       <c r="G298" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Popcorn", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Popcorn", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍿' },</v>
       </c>
     </row>
     <row r="299" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7825,10 +8238,12 @@
       </c>
       <c r="D299" s="2"/>
       <c r="E299" s="2"/>
-      <c r="F299" s="2"/>
+      <c r="F299" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="G299" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Corn Thins", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Corn Thins", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🌽' },</v>
       </c>
     </row>
     <row r="300" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7843,10 +8258,12 @@
       </c>
       <c r="D300" s="2"/>
       <c r="E300" s="2"/>
-      <c r="F300" s="2"/>
+      <c r="F300" s="2" t="s">
+        <v>427</v>
+      </c>
       <c r="G300" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Corn Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Corn Chips", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🌽' },</v>
       </c>
     </row>
     <row r="301" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7861,10 +8278,12 @@
       </c>
       <c r="D301" s="2"/>
       <c r="E301" s="2"/>
-      <c r="F301" s="2"/>
+      <c r="F301" s="2" t="s">
+        <v>508</v>
+      </c>
       <c r="G301" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Rice Cakes", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rice Cakes", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍥' },</v>
       </c>
     </row>
     <row r="302" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7879,10 +8298,12 @@
       </c>
       <c r="D302" s="2"/>
       <c r="E302" s="2"/>
-      <c r="F302" s="2"/>
+      <c r="F302" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="G302" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Crackers", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Crackers", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍘' },</v>
       </c>
     </row>
     <row r="303" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7897,10 +8318,12 @@
       </c>
       <c r="D303" s="2"/>
       <c r="E303" s="2"/>
-      <c r="F303" s="2"/>
+      <c r="F303" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="G303" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Cruskits", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Cruskits", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "", notes: "", emoji: '🍘' },</v>
       </c>
     </row>
     <row r="304" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7917,10 +8340,12 @@
         <v>330</v>
       </c>
       <c r="E304" s="2"/>
-      <c r="F304" s="2"/>
+      <c r="F304" s="2" t="s">
+        <v>482</v>
+      </c>
       <c r="G304" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Sweet &amp; Plain Biscuits/Cookies", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "2 pieces", notes: "", emoji: '' },</v>
+        <v>{ name: "Sweet &amp; Plain Biscuits/Cookies", category: "Snack Foods &amp; Confectionery", avoid: false, measurement: "2 pieces", notes: "", emoji: '🍪' },</v>
       </c>
     </row>
     <row r="305" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7935,10 +8360,12 @@
       </c>
       <c r="D305" s="2"/>
       <c r="E305" s="2"/>
-      <c r="F305" s="2"/>
+      <c r="F305" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G305" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Milk Chocolate", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Milk Chocolate", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="306" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7955,10 +8382,12 @@
         <v>333</v>
       </c>
       <c r="E306" s="2"/>
-      <c r="F306" s="2"/>
+      <c r="F306" s="2" t="s">
+        <v>475</v>
+      </c>
       <c r="G306" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "White Chocolate", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "&gt; 2 squares", notes: "", emoji: '' },</v>
+        <v>{ name: "White Chocolate", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "&gt; 2 squares", notes: "", emoji: '🍫' },</v>
       </c>
     </row>
     <row r="307" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7975,10 +8404,12 @@
       <c r="E307" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F307" s="2"/>
+      <c r="F307" s="2" t="s">
+        <v>484</v>
+      </c>
       <c r="G307" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Cup-a-Soup", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Cup-a-Soup", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '🍲' },</v>
       </c>
     </row>
     <row r="308" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7995,10 +8426,12 @@
       <c r="E308" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F308" s="2"/>
+      <c r="F308" s="2" t="s">
+        <v>480</v>
+      </c>
       <c r="G308" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Instant Noodles", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Instant Noodles", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '🍜' },</v>
       </c>
     </row>
     <row r="309" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8015,10 +8448,12 @@
       <c r="E309" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F309" s="2"/>
+      <c r="F309" s="2" t="s">
+        <v>509</v>
+      </c>
       <c r="G309" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Chips/Crackers", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Chips/Crackers", category: "Snack Foods &amp; Confectionery", avoid: true, measurement: "", notes: "No onion or garlic.", emoji: '🍘' },</v>
       </c>
     </row>
     <row r="310" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8035,10 +8470,12 @@
         <v>444</v>
       </c>
       <c r="E310" s="2"/>
-      <c r="F310" s="2"/>
+      <c r="F310" s="2" t="s">
+        <v>510</v>
+      </c>
       <c r="G310" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Almond Butter", category: "Condiments", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Almond Butter", category: "Condiments", avoid: false, measurement: "1 tablespoon", notes: "", emoji: '🧈' },</v>
       </c>
     </row>
     <row r="311" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8055,10 +8492,12 @@
       <c r="E311" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F311" s="2"/>
+      <c r="F311" s="2" t="s">
+        <v>430</v>
+      </c>
       <c r="G311" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Eggplant Dip", category: "Condiments", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Eggplant Dip", category: "Condiments", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '🍆' },</v>
       </c>
     </row>
     <row r="312" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8073,10 +8512,13 @@
       </c>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
-      <c r="F312" s="2"/>
+      <c r="F312" s="2" t="str">
+        <f>"🐟"</f>
+        <v>🐟</v>
+      </c>
       <c r="G312" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Fish Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fish Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🐟' },</v>
       </c>
     </row>
     <row r="313" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8093,10 +8535,12 @@
       <c r="E313" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F313" s="2"/>
+      <c r="F313" s="2" t="s">
+        <v>511</v>
+      </c>
       <c r="G313" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Herbs &amp; Spices", category: "Condiments", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '' },</v>
+        <v>{ name: "Herbs &amp; Spices", category: "Condiments", avoid: false, measurement: "", notes: "No onion or garlic.", emoji: '🌿' },</v>
       </c>
     </row>
     <row r="314" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8111,10 +8555,12 @@
       </c>
       <c r="D314" s="2"/>
       <c r="E314" s="2"/>
-      <c r="F314" s="2"/>
+      <c r="F314" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="G314" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Strawberry Jam", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Strawberry Jam", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍓' },</v>
       </c>
     </row>
     <row r="315" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8129,10 +8575,12 @@
       </c>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
-      <c r="F315" s="2"/>
+      <c r="F315" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="G315" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Raspberry Jam", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Raspberry Jam", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍓' },</v>
       </c>
     </row>
     <row r="316" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8147,10 +8595,12 @@
       </c>
       <c r="D316" s="2"/>
       <c r="E316" s="2"/>
-      <c r="F316" s="2"/>
+      <c r="F316" s="2" t="s">
+        <v>456</v>
+      </c>
       <c r="G316" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Marmalade", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Marmalade", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="317" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8165,10 +8615,13 @@
       </c>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
-      <c r="F317" s="2"/>
+      <c r="F317" s="2" t="str">
+        <f>"🖤"</f>
+        <v>🖤</v>
+      </c>
       <c r="G317" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Vegemite", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Vegemite", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🖤' },</v>
       </c>
     </row>
     <row r="318" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8183,10 +8636,12 @@
       </c>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
-      <c r="F318" s="2"/>
+      <c r="F318" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="G318" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Mayonnaise", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mayonnaise", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🥚' },</v>
       </c>
     </row>
     <row r="319" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8201,10 +8656,12 @@
       </c>
       <c r="D319" s="2"/>
       <c r="E319" s="2"/>
-      <c r="F319" s="2"/>
+      <c r="F319" s="2" t="s">
+        <v>504</v>
+      </c>
       <c r="G319" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Mint Jelly", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mint Jelly", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍮' },</v>
       </c>
     </row>
     <row r="320" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8219,10 +8676,12 @@
       </c>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
-      <c r="F320" s="2"/>
+      <c r="F320" s="2" t="s">
+        <v>484</v>
+      </c>
       <c r="G320" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Miso Paste", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Miso Paste", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍲' },</v>
       </c>
     </row>
     <row r="321" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8237,10 +8696,12 @@
       </c>
       <c r="D321" s="2"/>
       <c r="E321" s="2"/>
-      <c r="F321" s="2"/>
+      <c r="F321" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G321" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Mustard", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mustard", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="322" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8255,10 +8716,12 @@
       </c>
       <c r="D322" s="2"/>
       <c r="E322" s="2"/>
-      <c r="F322" s="2"/>
+      <c r="F322" s="2" t="s">
+        <v>514</v>
+      </c>
       <c r="G322" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>{ name: "Oyster Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Oyster Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🦪' },</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8273,10 +8736,12 @@
       </c>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
-      <c r="F323" s="2"/>
+      <c r="F323" s="2" t="s">
+        <v>492</v>
+      </c>
       <c r="G323" s="2" t="str">
         <f t="shared" ref="G323:G377" si="5">CONCATENATE("{ name: "&amp;CHAR(34),A323 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B323&amp;CHAR(34), ", ", "avoid: ", LOWER(C323), ", measurement: "&amp;CHAR(34), D323, CHAR(34), ", notes: ", CHAR(34), E323, CHAR(34), ", emoji: '", F323, "'", " },")</f>
-        <v>{ name: "Peanut Butter", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Peanut Butter", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🥜' },</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8291,10 +8756,12 @@
       </c>
       <c r="D324" s="2"/>
       <c r="E324" s="2"/>
-      <c r="F324" s="2"/>
+      <c r="F324" s="2" t="s">
+        <v>512</v>
+      </c>
       <c r="G324" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Remoulade", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Remoulade", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🥚' },</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8309,10 +8776,12 @@
       </c>
       <c r="D325" s="2"/>
       <c r="E325" s="2"/>
-      <c r="F325" s="2"/>
+      <c r="F325" s="2" t="s">
+        <v>515</v>
+      </c>
       <c r="G325" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Shrimp Paste", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Shrimp Paste", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🦐' },</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8327,10 +8796,12 @@
       </c>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
-      <c r="F326" s="2"/>
+      <c r="F326" s="2" t="s">
+        <v>516</v>
+      </c>
       <c r="G326" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Spirulina", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Spirulina", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🟢' },</v>
       </c>
     </row>
     <row r="327" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8345,10 +8816,12 @@
       </c>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
-      <c r="F327" s="2"/>
+      <c r="F327" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G327" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Soy Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Soy Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8365,10 +8838,12 @@
       <c r="E328" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="F328" s="2"/>
+      <c r="F328" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G328" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Sweet and Sour Sauce", category: "Condiments", avoid: false, measurement: "", notes: "No garlic.", emoji: '' },</v>
+        <v>{ name: "Sweet and Sour Sauce", category: "Condiments", avoid: false, measurement: "", notes: "No garlic.", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="329" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8385,10 +8860,12 @@
         <v>449</v>
       </c>
       <c r="E329" s="2"/>
-      <c r="F329" s="2"/>
+      <c r="F329" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="G329" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Tomato &amp; BBQ Sauce", category: "Condiments", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '' },</v>
+        <v>{ name: "Tomato &amp; BBQ Sauce", category: "Condiments", avoid: false, measurement: "2 tablespoons", notes: "", emoji: '🍅' },</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8403,10 +8880,12 @@
       </c>
       <c r="D330" s="2"/>
       <c r="E330" s="2"/>
-      <c r="F330" s="2"/>
+      <c r="F330" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G330" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Worcestershire Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Worcestershire Sauce", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="331" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8421,10 +8900,12 @@
       </c>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
-      <c r="F331" s="2"/>
+      <c r="F331" s="2" t="s">
+        <v>489</v>
+      </c>
       <c r="G331" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Vanilla Essence", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Vanilla Essence", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🍦' },</v>
       </c>
     </row>
     <row r="332" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8439,10 +8920,12 @@
       </c>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
-      <c r="F332" s="2"/>
+      <c r="F332" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G332" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Vinegar", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Vinegar", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="333" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8457,10 +8940,12 @@
       </c>
       <c r="D333" s="2"/>
       <c r="E333" s="2"/>
-      <c r="F333" s="2"/>
+      <c r="F333" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G333" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Mirin", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mirin", category: "Condiments", avoid: false, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="334" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8475,10 +8960,12 @@
       </c>
       <c r="D334" s="2"/>
       <c r="E334" s="2"/>
-      <c r="F334" s="2"/>
+      <c r="F334" s="2" t="s">
+        <v>517</v>
+      </c>
       <c r="G334" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Gravy Mix", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Gravy Mix", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🪦' },</v>
       </c>
     </row>
     <row r="335" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8493,10 +8980,12 @@
       </c>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
-      <c r="F335" s="2"/>
+      <c r="F335" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G335" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Marinades", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Marinades", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="336" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8511,10 +9000,12 @@
       </c>
       <c r="D336" s="2"/>
       <c r="E336" s="2"/>
-      <c r="F336" s="2"/>
+      <c r="F336" s="2" t="s">
+        <v>478</v>
+      </c>
       <c r="G336" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Pasta Sauce", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pasta Sauce", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🍝' },</v>
       </c>
     </row>
     <row r="337" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8529,10 +9020,12 @@
       </c>
       <c r="D337" s="2"/>
       <c r="E337" s="2"/>
-      <c r="F337" s="2"/>
+      <c r="F337" s="2" t="s">
+        <v>518</v>
+      </c>
       <c r="G337" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Curry Paste", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Curry Paste", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🍛' },</v>
       </c>
     </row>
     <row r="338" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8547,10 +9040,12 @@
       </c>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
-      <c r="F338" s="2"/>
+      <c r="F338" s="2" t="s">
+        <v>519</v>
+      </c>
       <c r="G338" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Honey", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Honey", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🍯' },</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8567,10 +9062,12 @@
         <v>445</v>
       </c>
       <c r="E339" s="2"/>
-      <c r="F339" s="2"/>
+      <c r="F339" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G339" s="2" t="str">
         <f>CONCATENATE("{ name: "&amp;CHAR(34),A339 &amp;CHAR(34), ", ", "category: "&amp;CHAR(34), B339&amp;CHAR(34), ", ", "avoid: ", LOWER(C339), ", measurement: "&amp;CHAR(34), D339, CHAR(34), ", notes: ", CHAR(34), E339, CHAR(34), ", emoji: '", F339, "'", " },")</f>
-        <v>{ name: "Hummus", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Hummus", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8585,10 +9082,12 @@
       </c>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
-      <c r="F340" s="2"/>
+      <c r="F340" s="2" t="s">
+        <v>520</v>
+      </c>
       <c r="G340" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Seasoning Mixes", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Seasoning Mixes", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🧂' },</v>
       </c>
     </row>
     <row r="341" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8603,10 +9102,12 @@
       </c>
       <c r="D341" s="2"/>
       <c r="E341" s="2"/>
-      <c r="F341" s="2"/>
+      <c r="F341" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G341" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Relish and Chutney", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Relish and Chutney", category: "Condiments", avoid: true, measurement: "", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="342" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8623,10 +9124,12 @@
         <v>445</v>
       </c>
       <c r="E342" s="2"/>
-      <c r="F342" s="2"/>
+      <c r="F342" s="2" t="s">
+        <v>513</v>
+      </c>
       <c r="G342" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Tahini", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '' },</v>
+        <v>{ name: "Tahini", category: "Condiments", avoid: true, measurement: "&gt; 1 tablespoon", notes: "", emoji: '🫙' },</v>
       </c>
     </row>
     <row r="343" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8643,10 +9146,12 @@
         <v>372</v>
       </c>
       <c r="E343" s="2"/>
-      <c r="F343" s="2"/>
+      <c r="F343" s="2" t="s">
+        <v>481</v>
+      </c>
       <c r="G343" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Cranberry Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Cranberry Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '🧃' },</v>
       </c>
     </row>
     <row r="344" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8663,10 +9168,12 @@
         <v>372</v>
       </c>
       <c r="E344" s="2"/>
-      <c r="F344" s="2"/>
+      <c r="F344" s="2" t="s">
+        <v>439</v>
+      </c>
       <c r="G344" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Tomato Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Tomato Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '🍅' },</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8683,10 +9190,12 @@
         <v>372</v>
       </c>
       <c r="E345" s="2"/>
-      <c r="F345" s="2"/>
+      <c r="F345" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="G345" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Lime Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Lime Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '🍋' },</v>
       </c>
     </row>
     <row r="346" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8703,10 +9212,12 @@
         <v>372</v>
       </c>
       <c r="E346" s="2"/>
-      <c r="F346" s="2"/>
+      <c r="F346" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="G346" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Lemon Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Lemon Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '🍋' },</v>
       </c>
     </row>
     <row r="347" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8723,10 +9234,12 @@
         <v>372</v>
       </c>
       <c r="E347" s="2"/>
-      <c r="F347" s="2"/>
+      <c r="F347" s="2" t="s">
+        <v>521</v>
+      </c>
       <c r="G347" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Spirulina Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Spirulina Juice", category: "Drinks", avoid: false, measurement: "1 cup", notes: "", emoji: '🥤' },</v>
       </c>
     </row>
     <row r="348" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8743,10 +9256,12 @@
         <v>10</v>
       </c>
       <c r="E348" s="5"/>
-      <c r="F348" s="5"/>
+      <c r="F348" s="5" t="s">
+        <v>456</v>
+      </c>
       <c r="G348" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Orange Juice (Fresh)", category: "Drinks", avoid: false, measurement: "½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Orange Juice (Fresh)", category: "Drinks", avoid: false, measurement: "½ cup", notes: "", emoji: '🍊' },</v>
       </c>
     </row>
     <row r="349" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8761,10 +9276,12 @@
       </c>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
-      <c r="F349" s="2"/>
+      <c r="F349" s="2" t="s">
+        <v>522</v>
+      </c>
       <c r="G349" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Coffee", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Coffee", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '☕' },</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8779,10 +9296,12 @@
       </c>
       <c r="D350" s="2"/>
       <c r="E350" s="2"/>
-      <c r="F350" s="2"/>
+      <c r="F350" s="2" t="s">
+        <v>523</v>
+      </c>
       <c r="G350" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Black Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Black Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍵' },</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8797,10 +9316,12 @@
       </c>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
-      <c r="F351" s="2"/>
+      <c r="F351" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G351" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Dandelion Tea (Weak)", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Dandelion Tea (Weak)", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="352" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8815,10 +9336,12 @@
       </c>
       <c r="D352" s="2"/>
       <c r="E352" s="2"/>
-      <c r="F352" s="2"/>
+      <c r="F352" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G352" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Peppermint Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Peppermint Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8833,10 +9356,12 @@
       </c>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
-      <c r="F353" s="2"/>
+      <c r="F353" s="2" t="s">
+        <v>523</v>
+      </c>
       <c r="G353" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Green Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Green Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍵' },</v>
       </c>
     </row>
     <row r="354" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8851,10 +9376,12 @@
       </c>
       <c r="D354" s="2"/>
       <c r="E354" s="2"/>
-      <c r="F354" s="2"/>
+      <c r="F354" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G354" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Rooibos Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rooibos Tea", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8869,10 +9396,12 @@
       </c>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
-      <c r="F355" s="2"/>
+      <c r="F355" s="2" t="s">
+        <v>525</v>
+      </c>
       <c r="G355" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Beer", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Beer", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍺' },</v>
       </c>
     </row>
     <row r="356" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8887,10 +9416,12 @@
       </c>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
-      <c r="F356" s="2"/>
+      <c r="F356" s="2" t="s">
+        <v>526</v>
+      </c>
       <c r="G356" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Whiskey", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Whiskey", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🥃' },</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8905,10 +9436,12 @@
       </c>
       <c r="D357" s="2"/>
       <c r="E357" s="2"/>
-      <c r="F357" s="2"/>
+      <c r="F357" s="2" t="s">
+        <v>527</v>
+      </c>
       <c r="G357" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Gin", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Gin", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍶' },</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8923,10 +9456,12 @@
       </c>
       <c r="D358" s="2"/>
       <c r="E358" s="2"/>
-      <c r="F358" s="2"/>
+      <c r="F358" s="2" t="s">
+        <v>527</v>
+      </c>
       <c r="G358" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Vodka", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Vodka", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍶' },</v>
       </c>
     </row>
     <row r="359" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8941,10 +9476,12 @@
       </c>
       <c r="D359" s="2"/>
       <c r="E359" s="2"/>
-      <c r="F359" s="2"/>
+      <c r="F359" s="2" t="s">
+        <v>528</v>
+      </c>
       <c r="G359" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Champagne", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Champagne", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍾' },</v>
       </c>
     </row>
     <row r="360" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8959,10 +9496,12 @@
       </c>
       <c r="D360" s="2"/>
       <c r="E360" s="2"/>
-      <c r="F360" s="2"/>
+      <c r="F360" s="2" t="s">
+        <v>529</v>
+      </c>
       <c r="G360" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Red Wine", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Red Wine", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍷' },</v>
       </c>
     </row>
     <row r="361" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8977,10 +9516,12 @@
       </c>
       <c r="D361" s="2"/>
       <c r="E361" s="2"/>
-      <c r="F361" s="2"/>
+      <c r="F361" s="2" t="s">
+        <v>529</v>
+      </c>
       <c r="G361" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "White Wine", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "White Wine", category: "Drinks", avoid: false, measurement: "", notes: "", emoji: '🍷' },</v>
       </c>
     </row>
     <row r="362" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8997,10 +9538,12 @@
         <v>238</v>
       </c>
       <c r="E362" s="5"/>
-      <c r="F362" s="5"/>
+      <c r="F362" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="G362" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Coconut Water", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Coconut Water", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '🥥' },</v>
       </c>
     </row>
     <row r="363" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9015,10 +9558,12 @@
       </c>
       <c r="D363" s="2"/>
       <c r="E363" s="2"/>
-      <c r="F363" s="2"/>
+      <c r="F363" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="G363" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Apple Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Apple Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍏' },</v>
       </c>
     </row>
     <row r="364" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9033,10 +9578,12 @@
       </c>
       <c r="D364" s="2"/>
       <c r="E364" s="2"/>
-      <c r="F364" s="2"/>
+      <c r="F364" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="G364" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Mango Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Mango Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🥭' },</v>
       </c>
     </row>
     <row r="365" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9051,10 +9598,12 @@
       </c>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
-      <c r="F365" s="2"/>
+      <c r="F365" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="G365" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Pear Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pear Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍐' },</v>
       </c>
     </row>
     <row r="366" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9071,10 +9620,12 @@
         <v>238</v>
       </c>
       <c r="E366" s="5"/>
-      <c r="F366" s="5"/>
+      <c r="F366" s="5" t="s">
+        <v>530</v>
+      </c>
       <c r="G366" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Kombucha", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '' },</v>
+        <v>{ name: "Kombucha", category: "Drinks", avoid: true, measurement: "&gt; ½ cup", notes: "", emoji: '🍹' },</v>
       </c>
     </row>
     <row r="367" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9089,10 +9640,12 @@
       </c>
       <c r="D367" s="2"/>
       <c r="E367" s="2"/>
-      <c r="F367" s="2"/>
+      <c r="F367" s="2" t="s">
+        <v>531</v>
+      </c>
       <c r="G367" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Milk Drinks", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Milk Drinks", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🧋' },</v>
       </c>
     </row>
     <row r="368" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9107,10 +9660,12 @@
       </c>
       <c r="D368" s="2"/>
       <c r="E368" s="2"/>
-      <c r="F368" s="2"/>
+      <c r="F368" s="2" t="s">
+        <v>481</v>
+      </c>
       <c r="G368" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Pomegranate Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pomegranate Juice", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🧃' },</v>
       </c>
     </row>
     <row r="369" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9125,10 +9680,12 @@
       </c>
       <c r="D369" s="2"/>
       <c r="E369" s="2"/>
-      <c r="F369" s="2"/>
+      <c r="F369" s="2" t="s">
+        <v>523</v>
+      </c>
       <c r="G369" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Chamomile Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Chamomile Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍵' },</v>
       </c>
     </row>
     <row r="370" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9143,10 +9700,12 @@
       </c>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
-      <c r="F370" s="2"/>
+      <c r="F370" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G370" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Dandelion Tea (Strong)", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Dandelion Tea (Strong)", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="371" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9161,10 +9720,12 @@
       </c>
       <c r="D371" s="2"/>
       <c r="E371" s="2"/>
-      <c r="F371" s="2"/>
+      <c r="F371" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G371" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Fennel Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Fennel Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="372" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9179,10 +9740,12 @@
       </c>
       <c r="D372" s="2"/>
       <c r="E372" s="2"/>
-      <c r="F372" s="2"/>
+      <c r="F372" s="2" t="s">
+        <v>523</v>
+      </c>
       <c r="G372" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Oolong Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Oolong Tea", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍵' },</v>
       </c>
     </row>
     <row r="373" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9197,10 +9760,12 @@
       </c>
       <c r="D373" s="2"/>
       <c r="E373" s="2"/>
-      <c r="F373" s="2"/>
+      <c r="F373" s="2" t="s">
+        <v>524</v>
+      </c>
       <c r="G373" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Chai Tea (Powders)", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Chai Tea (Powders)", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🫖' },</v>
       </c>
     </row>
     <row r="374" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9215,10 +9780,12 @@
       </c>
       <c r="D374" s="2"/>
       <c r="E374" s="2"/>
-      <c r="F374" s="2"/>
+      <c r="F374" s="2" t="s">
+        <v>526</v>
+      </c>
       <c r="G374" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Rum", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Rum", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🥃' },</v>
       </c>
     </row>
     <row r="375" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9233,10 +9800,12 @@
       </c>
       <c r="D375" s="2"/>
       <c r="E375" s="2"/>
-      <c r="F375" s="2"/>
+      <c r="F375" s="2" t="s">
+        <v>529</v>
+      </c>
       <c r="G375" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Dessert Wine", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Dessert Wine", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍷' },</v>
       </c>
     </row>
     <row r="376" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9251,10 +9820,12 @@
       </c>
       <c r="D376" s="2"/>
       <c r="E376" s="2"/>
-      <c r="F376" s="2"/>
+      <c r="F376" s="2" t="s">
+        <v>525</v>
+      </c>
       <c r="G376" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Apple Cider", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Apple Cider", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍺' },</v>
       </c>
     </row>
     <row r="377" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9269,10 +9840,12 @@
       </c>
       <c r="D377" s="2"/>
       <c r="E377" s="2"/>
-      <c r="F377" s="2"/>
+      <c r="F377" s="2" t="s">
+        <v>525</v>
+      </c>
       <c r="G377" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>{ name: "Pear Cider", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '' },</v>
+        <v>{ name: "Pear Cider", category: "Drinks", avoid: true, measurement: "", notes: "", emoji: '🍺' },</v>
       </c>
     </row>
   </sheetData>

</xml_diff>